<commit_message>
Auto-committed on 2022/03/07 週一
</commit_message>
<xml_diff>
--- a/Program/Other/LY003_底稿_非RBC_表14-2_會計部年度檢查報表.xlsx
+++ b/Program/Other/LY003_底稿_非RBC_表14-2_會計部年度檢查報表.xlsx
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="150">
   <si>
     <r>
       <t>新光人壽保險股份有限公司</t>
@@ -1609,6 +1609,22 @@
     <t>資產分類
 法定備呆金額</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>上年度業主權益</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3515,7 +3531,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3765,11 +3781,111 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="37" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="4" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="181" fontId="4" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="181" fontId="4" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3809,105 +3925,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="12" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="12" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="37" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="288">
@@ -6956,8 +6981,8 @@
   </sheetPr>
   <dimension ref="A1:Y116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="K83" sqref="K83"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71:J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
@@ -6997,11 +7022,11 @@
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -7015,39 +7040,39 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:13" s="7" customFormat="1">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="103" t="s">
+      <c r="C3" s="130"/>
+      <c r="D3" s="135" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="114" t="s">
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="105" t="s">
+      <c r="H3" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="105" t="s">
+      <c r="I3" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="107" t="s">
+      <c r="J3" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="109" t="s">
+      <c r="K3" s="116" t="s">
         <v>10</v>
       </c>
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:13" s="7" customFormat="1">
-      <c r="A4" s="96"/>
-      <c r="B4" s="99"/>
-      <c r="C4" s="100"/>
+      <c r="A4" s="128"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="132"/>
       <c r="D4" s="10" t="s">
         <v>11</v>
       </c>
@@ -7057,17 +7082,17 @@
       <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="115"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="108"/>
-      <c r="K4" s="110"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="117"/>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:13" s="7" customFormat="1">
-      <c r="A5" s="96"/>
-      <c r="B5" s="101"/>
-      <c r="C5" s="102"/>
+      <c r="A5" s="128"/>
+      <c r="B5" s="133"/>
+      <c r="C5" s="134"/>
       <c r="D5" s="12" t="s">
         <v>14</v>
       </c>
@@ -7099,7 +7124,7 @@
       <c r="A6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="118" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -7113,11 +7138,11 @@
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="21"/>
-      <c r="I6" s="124" t="e">
-        <f t="shared" ref="I6:J7" si="0">H6/$L$7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J6" s="124" t="e">
+      <c r="I6" s="91" t="e">
+        <f t="shared" ref="I6:I7" si="0">H6/$L$7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J6" s="91" t="e">
         <f>I6/$L$6</f>
         <v>#DIV/0!</v>
       </c>
@@ -7133,7 +7158,7 @@
       <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="112"/>
+      <c r="B7" s="119"/>
       <c r="C7" s="17" t="s">
         <v>27</v>
       </c>
@@ -7151,11 +7176,11 @@
       <c r="H7" s="24">
         <v>0</v>
       </c>
-      <c r="I7" s="124" t="e">
+      <c r="I7" s="91" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J7" s="124" t="e">
+      <c r="J7" s="91" t="e">
         <f>I7/$L$6</f>
         <v>#DIV/0!</v>
       </c>
@@ -7171,7 +7196,7 @@
       <c r="A8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="92"/>
+      <c r="B8" s="120"/>
       <c r="C8" s="26" t="s">
         <v>30</v>
       </c>
@@ -7183,23 +7208,25 @@
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="28"/>
-      <c r="I8" s="124" t="e">
+      <c r="I8" s="91" t="e">
         <f>H8/$L$7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J8" s="124" t="e">
+      <c r="J8" s="91" t="e">
         <f t="shared" ref="I8:J69" si="2">I8/$L$6</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K8" s="20"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="15"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="25" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="9" spans="1:13" s="7" customFormat="1">
       <c r="A9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="92"/>
+      <c r="B9" s="120"/>
       <c r="C9" s="26" t="s">
         <v>32</v>
       </c>
@@ -7211,11 +7238,11 @@
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="28"/>
-      <c r="I9" s="124" t="e">
+      <c r="I9" s="91" t="e">
         <f t="shared" ref="I9:I68" si="3">H9/$L$7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J9" s="124" t="e">
+      <c r="J9" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7226,7 +7253,7 @@
       <c r="A10" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="92"/>
+      <c r="B10" s="120"/>
       <c r="C10" s="26" t="s">
         <v>34</v>
       </c>
@@ -7238,11 +7265,11 @@
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="28"/>
-      <c r="I10" s="124" t="e">
+      <c r="I10" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J10" s="124" t="e">
+      <c r="J10" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7253,7 +7280,7 @@
       <c r="A11" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="92"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="26" t="s">
         <v>36</v>
       </c>
@@ -7265,11 +7292,11 @@
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="27"/>
-      <c r="I11" s="124" t="e">
+      <c r="I11" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J11" s="124" t="e">
+      <c r="J11" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7280,7 +7307,7 @@
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="92"/>
+      <c r="B12" s="120"/>
       <c r="C12" s="32" t="s">
         <v>38</v>
       </c>
@@ -7292,11 +7319,11 @@
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="27"/>
-      <c r="I12" s="124" t="e">
+      <c r="I12" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J12" s="124" t="e">
+      <c r="J12" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7307,7 +7334,7 @@
       <c r="A13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="92"/>
+      <c r="B13" s="120"/>
       <c r="C13" s="32" t="s">
         <v>40</v>
       </c>
@@ -7328,11 +7355,11 @@
         <f>SUM(H6:H12)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="124" t="e">
+      <c r="I13" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J13" s="124" t="e">
+      <c r="J13" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7343,25 +7370,25 @@
       <c r="A14" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="121" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="125"/>
-      <c r="E14" s="125"/>
-      <c r="F14" s="126" t="e">
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G14" s="127"/>
+      <c r="G14" s="94"/>
       <c r="H14" s="28"/>
-      <c r="I14" s="124" t="e">
+      <c r="I14" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J14" s="124" t="e">
+      <c r="J14" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7372,23 +7399,23 @@
       <c r="A15" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="92"/>
+      <c r="B15" s="120"/>
       <c r="C15" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="128"/>
+      <c r="D15" s="95"/>
       <c r="E15" s="35"/>
-      <c r="F15" s="126" t="e">
+      <c r="F15" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="129"/>
+      <c r="G15" s="96"/>
       <c r="H15" s="36"/>
-      <c r="I15" s="124" t="e">
+      <c r="I15" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J15" s="124" t="e">
+      <c r="J15" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7399,23 +7426,23 @@
       <c r="A16" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="92"/>
+      <c r="B16" s="120"/>
       <c r="C16" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="125"/>
-      <c r="E16" s="125"/>
-      <c r="F16" s="126" t="e">
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G16" s="129"/>
+      <c r="G16" s="96"/>
       <c r="H16" s="28"/>
-      <c r="I16" s="124" t="e">
+      <c r="I16" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J16" s="124" t="e">
+      <c r="J16" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7426,23 +7453,23 @@
       <c r="A17" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="113"/>
+      <c r="B17" s="122"/>
       <c r="C17" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="125"/>
-      <c r="E17" s="125"/>
-      <c r="F17" s="126" t="e">
+      <c r="D17" s="92"/>
+      <c r="E17" s="92"/>
+      <c r="F17" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="129"/>
+      <c r="G17" s="96"/>
       <c r="H17" s="28"/>
-      <c r="I17" s="124" t="e">
+      <c r="I17" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J17" s="124" t="e">
+      <c r="J17" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7452,7 +7479,7 @@
       <c r="A18" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="113"/>
+      <c r="B18" s="122"/>
       <c r="C18" s="37" t="s">
         <v>40</v>
       </c>
@@ -7464,20 +7491,20 @@
         <f>SUM(E14:E17)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="126" t="e">
+      <c r="F18" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="129"/>
+      <c r="G18" s="96"/>
       <c r="H18" s="30">
         <f>SUM(H14:H17)</f>
         <v>0</v>
       </c>
-      <c r="I18" s="124" t="e">
+      <c r="I18" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J18" s="124" t="e">
+      <c r="J18" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7487,7 +7514,7 @@
       <c r="A19" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="91" t="s">
+      <c r="B19" s="121" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="26" t="s">
@@ -7495,17 +7522,17 @@
       </c>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
-      <c r="F19" s="126" t="e">
+      <c r="F19" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="129"/>
+      <c r="G19" s="96"/>
       <c r="H19" s="30"/>
-      <c r="I19" s="124" t="e">
+      <c r="I19" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J19" s="124" t="e">
+      <c r="J19" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7515,23 +7542,23 @@
       <c r="A20" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="92"/>
+      <c r="B20" s="120"/>
       <c r="C20" s="26" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
-      <c r="F20" s="126" t="e">
+      <c r="F20" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="129"/>
+      <c r="G20" s="96"/>
       <c r="H20" s="30"/>
-      <c r="I20" s="124" t="e">
+      <c r="I20" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J20" s="124" t="e">
+      <c r="J20" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7541,23 +7568,23 @@
       <c r="A21" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="92"/>
+      <c r="B21" s="120"/>
       <c r="C21" s="26" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="30"/>
       <c r="E21" s="30"/>
-      <c r="F21" s="126" t="e">
+      <c r="F21" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G21" s="129"/>
+      <c r="G21" s="96"/>
       <c r="H21" s="30"/>
-      <c r="I21" s="124" t="e">
+      <c r="I21" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J21" s="124" t="e">
+      <c r="J21" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7567,23 +7594,23 @@
       <c r="A22" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="92"/>
+      <c r="B22" s="120"/>
       <c r="C22" s="37" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
-      <c r="F22" s="126" t="e">
+      <c r="F22" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G22" s="129"/>
+      <c r="G22" s="96"/>
       <c r="H22" s="30"/>
-      <c r="I22" s="124" t="e">
+      <c r="I22" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J22" s="124" t="e">
+      <c r="J22" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7593,7 +7620,7 @@
       <c r="A23" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="121" t="s">
+      <c r="B23" s="109" t="s">
         <v>57</v>
       </c>
       <c r="C23" s="37" t="s">
@@ -7607,20 +7634,20 @@
         <f>SUM(E19:E22)</f>
         <v>0</v>
       </c>
-      <c r="F23" s="126" t="e">
+      <c r="F23" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G23" s="129"/>
+      <c r="G23" s="96"/>
       <c r="H23" s="30">
         <f>SUM(H19:H22)</f>
         <v>0</v>
       </c>
-      <c r="I23" s="124" t="e">
+      <c r="I23" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J23" s="124" t="e">
+      <c r="J23" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7630,23 +7657,23 @@
       <c r="A24" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="122"/>
+      <c r="B24" s="110"/>
       <c r="C24" s="37" t="s">
         <v>60</v>
       </c>
       <c r="D24" s="30"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="126" t="e">
+      <c r="F24" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="129"/>
+      <c r="G24" s="96"/>
       <c r="H24" s="21"/>
-      <c r="I24" s="124" t="e">
+      <c r="I24" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J24" s="124" t="e">
+      <c r="J24" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7656,7 +7683,7 @@
       <c r="A25" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="121" t="s">
+      <c r="B25" s="109" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="26" t="s">
@@ -7670,20 +7697,20 @@
         <f>SUM(E26:E30)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="126" t="e">
+      <c r="F25" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G25" s="129"/>
+      <c r="G25" s="96"/>
       <c r="H25" s="30">
         <f>SUM(H26:H30)</f>
         <v>0</v>
       </c>
-      <c r="I25" s="124" t="e">
+      <c r="I25" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J25" s="124" t="e">
+      <c r="J25" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7693,23 +7720,23 @@
       <c r="A26" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="123"/>
+      <c r="B26" s="111"/>
       <c r="C26" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D26" s="30"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="126" t="e">
+      <c r="E26" s="97"/>
+      <c r="F26" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G26" s="129"/>
+      <c r="G26" s="96"/>
       <c r="H26" s="39"/>
-      <c r="I26" s="124" t="e">
+      <c r="I26" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J26" s="124" t="e">
+      <c r="J26" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7719,23 +7746,23 @@
       <c r="A27" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="123"/>
+      <c r="B27" s="111"/>
       <c r="C27" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D27" s="30"/>
       <c r="E27" s="30"/>
-      <c r="F27" s="126" t="e">
+      <c r="F27" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G27" s="129"/>
+      <c r="G27" s="96"/>
       <c r="H27" s="21"/>
-      <c r="I27" s="124" t="e">
+      <c r="I27" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J27" s="124" t="e">
+      <c r="J27" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7745,23 +7772,23 @@
       <c r="A28" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="123"/>
+      <c r="B28" s="111"/>
       <c r="C28" s="38" t="s">
         <v>68</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
-      <c r="F28" s="126" t="e">
+      <c r="F28" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G28" s="129"/>
+      <c r="G28" s="96"/>
       <c r="H28" s="21"/>
-      <c r="I28" s="124" t="e">
+      <c r="I28" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J28" s="124" t="e">
+      <c r="J28" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7771,23 +7798,23 @@
       <c r="A29" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="123"/>
+      <c r="B29" s="111"/>
       <c r="C29" s="38" t="s">
         <v>70</v>
       </c>
       <c r="D29" s="30"/>
       <c r="E29" s="30"/>
-      <c r="F29" s="126" t="e">
+      <c r="F29" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G29" s="129"/>
+      <c r="G29" s="96"/>
       <c r="H29" s="21"/>
-      <c r="I29" s="124" t="e">
+      <c r="I29" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J29" s="124" t="e">
+      <c r="J29" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7797,23 +7824,23 @@
       <c r="A30" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="123"/>
+      <c r="B30" s="111"/>
       <c r="C30" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="30"/>
-      <c r="F30" s="126" t="e">
+      <c r="F30" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G30" s="129"/>
+      <c r="G30" s="96"/>
       <c r="H30" s="21"/>
-      <c r="I30" s="124" t="e">
+      <c r="I30" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J30" s="124" t="e">
+      <c r="J30" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7823,7 +7850,7 @@
       <c r="A31" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="123"/>
+      <c r="B31" s="111"/>
       <c r="C31" s="26" t="s">
         <v>27</v>
       </c>
@@ -7835,20 +7862,20 @@
         <f>SUM(E32:E36)</f>
         <v>0</v>
       </c>
-      <c r="F31" s="126" t="e">
+      <c r="F31" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G31" s="129"/>
+      <c r="G31" s="96"/>
       <c r="H31" s="30">
         <f>SUM(H32:H36)</f>
         <v>0</v>
       </c>
-      <c r="I31" s="124" t="e">
+      <c r="I31" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J31" s="124" t="e">
+      <c r="J31" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7858,23 +7885,23 @@
       <c r="A32" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="123"/>
+      <c r="B32" s="111"/>
       <c r="C32" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
-      <c r="F32" s="126" t="e">
+      <c r="F32" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G32" s="129"/>
+      <c r="G32" s="96"/>
       <c r="H32" s="24"/>
-      <c r="I32" s="124" t="e">
+      <c r="I32" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J32" s="124" t="e">
+      <c r="J32" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7884,23 +7911,23 @@
       <c r="A33" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="123"/>
+      <c r="B33" s="111"/>
       <c r="C33" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D33" s="30"/>
       <c r="E33" s="30"/>
-      <c r="F33" s="126" t="e">
+      <c r="F33" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G33" s="129"/>
+      <c r="G33" s="96"/>
       <c r="H33" s="24"/>
-      <c r="I33" s="124" t="e">
+      <c r="I33" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J33" s="124" t="e">
+      <c r="J33" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7911,23 +7938,23 @@
       <c r="A34" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="123"/>
+      <c r="B34" s="111"/>
       <c r="C34" s="38" t="s">
         <v>68</v>
       </c>
       <c r="D34" s="30"/>
       <c r="E34" s="30"/>
-      <c r="F34" s="126" t="e">
+      <c r="F34" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G34" s="129"/>
+      <c r="G34" s="96"/>
       <c r="H34" s="24"/>
-      <c r="I34" s="124" t="e">
+      <c r="I34" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J34" s="124" t="e">
+      <c r="J34" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7938,23 +7965,23 @@
       <c r="A35" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="123"/>
+      <c r="B35" s="111"/>
       <c r="C35" s="38" t="s">
         <v>70</v>
       </c>
       <c r="D35" s="30"/>
       <c r="E35" s="30"/>
-      <c r="F35" s="126" t="e">
+      <c r="F35" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G35" s="129"/>
+      <c r="G35" s="96"/>
       <c r="H35" s="28"/>
-      <c r="I35" s="124" t="e">
+      <c r="I35" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J35" s="124" t="e">
+      <c r="J35" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7965,23 +7992,23 @@
       <c r="A36" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="123"/>
+      <c r="B36" s="111"/>
       <c r="C36" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D36" s="30"/>
       <c r="E36" s="30"/>
-      <c r="F36" s="126" t="e">
+      <c r="F36" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G36" s="129"/>
+      <c r="G36" s="96"/>
       <c r="H36" s="28"/>
-      <c r="I36" s="124" t="e">
+      <c r="I36" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J36" s="124" t="e">
+      <c r="J36" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -7992,7 +8019,7 @@
       <c r="A37" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="123"/>
+      <c r="B37" s="111"/>
       <c r="C37" s="26" t="s">
         <v>30</v>
       </c>
@@ -8004,20 +8031,20 @@
         <f>SUM(E38:E42)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="126" t="e">
+      <c r="F37" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G37" s="129"/>
+      <c r="G37" s="96"/>
       <c r="H37" s="30">
         <f>SUM(H38:H42)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="124" t="e">
+      <c r="I37" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J37" s="124" t="e">
+      <c r="J37" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8028,23 +8055,23 @@
       <c r="A38" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="123"/>
+      <c r="B38" s="111"/>
       <c r="C38" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D38" s="30"/>
       <c r="E38" s="30"/>
-      <c r="F38" s="126" t="e">
+      <c r="F38" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G38" s="129"/>
+      <c r="G38" s="96"/>
       <c r="H38" s="30"/>
-      <c r="I38" s="124" t="e">
+      <c r="I38" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J38" s="124" t="e">
+      <c r="J38" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8055,23 +8082,23 @@
       <c r="A39" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="123"/>
+      <c r="B39" s="111"/>
       <c r="C39" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D39" s="30"/>
       <c r="E39" s="30"/>
-      <c r="F39" s="126" t="e">
+      <c r="F39" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G39" s="129"/>
+      <c r="G39" s="96"/>
       <c r="H39" s="30"/>
-      <c r="I39" s="124" t="e">
+      <c r="I39" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J39" s="124" t="e">
+      <c r="J39" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8082,23 +8109,23 @@
       <c r="A40" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="123"/>
+      <c r="B40" s="111"/>
       <c r="C40" s="38" t="s">
         <v>68</v>
       </c>
       <c r="D40" s="30"/>
       <c r="E40" s="30"/>
-      <c r="F40" s="126" t="e">
+      <c r="F40" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G40" s="129"/>
+      <c r="G40" s="96"/>
       <c r="H40" s="30"/>
-      <c r="I40" s="124" t="e">
+      <c r="I40" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J40" s="124" t="e">
+      <c r="J40" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8109,23 +8136,23 @@
       <c r="A41" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="123"/>
+      <c r="B41" s="111"/>
       <c r="C41" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="131"/>
+      <c r="D41" s="98"/>
       <c r="E41" s="28"/>
-      <c r="F41" s="126" t="e">
+      <c r="F41" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G41" s="129"/>
+      <c r="G41" s="96"/>
       <c r="H41" s="30"/>
-      <c r="I41" s="124" t="e">
+      <c r="I41" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J41" s="124" t="e">
+      <c r="J41" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8136,23 +8163,23 @@
       <c r="A42" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="123"/>
+      <c r="B42" s="111"/>
       <c r="C42" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="30"/>
-      <c r="F42" s="126" t="e">
+      <c r="F42" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G42" s="129"/>
+      <c r="G42" s="96"/>
       <c r="H42" s="30"/>
-      <c r="I42" s="124" t="e">
+      <c r="I42" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J42" s="124" t="e">
+      <c r="J42" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8163,7 +8190,7 @@
       <c r="A43" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="123"/>
+      <c r="B43" s="111"/>
       <c r="C43" s="26" t="s">
         <v>86</v>
       </c>
@@ -8175,20 +8202,20 @@
         <f>SUM(E44:E48)</f>
         <v>0</v>
       </c>
-      <c r="F43" s="126" t="e">
+      <c r="F43" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G43" s="129"/>
+      <c r="G43" s="96"/>
       <c r="H43" s="30">
         <f>SUM(H44:H48)</f>
         <v>0</v>
       </c>
-      <c r="I43" s="124" t="e">
+      <c r="I43" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J43" s="124" t="e">
+      <c r="J43" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8199,23 +8226,23 @@
       <c r="A44" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="123"/>
+      <c r="B44" s="111"/>
       <c r="C44" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="30"/>
-      <c r="F44" s="126" t="e">
+      <c r="F44" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G44" s="129"/>
+      <c r="G44" s="96"/>
       <c r="H44" s="30"/>
-      <c r="I44" s="124" t="e">
+      <c r="I44" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J44" s="124" t="e">
+      <c r="J44" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8226,23 +8253,23 @@
       <c r="A45" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="123"/>
+      <c r="B45" s="111"/>
       <c r="C45" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D45" s="30"/>
       <c r="E45" s="30"/>
-      <c r="F45" s="126" t="e">
+      <c r="F45" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G45" s="129"/>
+      <c r="G45" s="96"/>
       <c r="H45" s="24"/>
-      <c r="I45" s="124" t="e">
+      <c r="I45" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J45" s="124" t="e">
+      <c r="J45" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8253,23 +8280,23 @@
       <c r="A46" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="123"/>
+      <c r="B46" s="111"/>
       <c r="C46" s="38" t="s">
         <v>68</v>
       </c>
       <c r="D46" s="30"/>
       <c r="E46" s="30"/>
-      <c r="F46" s="126" t="e">
+      <c r="F46" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G46" s="129"/>
+      <c r="G46" s="96"/>
       <c r="H46" s="39"/>
-      <c r="I46" s="124" t="e">
+      <c r="I46" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J46" s="124" t="e">
+      <c r="J46" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8280,23 +8307,23 @@
       <c r="A47" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="123"/>
+      <c r="B47" s="111"/>
       <c r="C47" s="38" t="s">
         <v>70</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="30"/>
-      <c r="F47" s="126" t="e">
+      <c r="F47" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G47" s="129"/>
+      <c r="G47" s="96"/>
       <c r="H47" s="24"/>
-      <c r="I47" s="124" t="e">
+      <c r="I47" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J47" s="124" t="e">
+      <c r="J47" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8307,23 +8334,23 @@
       <c r="A48" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="123"/>
+      <c r="B48" s="111"/>
       <c r="C48" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D48" s="30"/>
       <c r="E48" s="30"/>
-      <c r="F48" s="126" t="e">
+      <c r="F48" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G48" s="129"/>
+      <c r="G48" s="96"/>
       <c r="H48" s="21"/>
-      <c r="I48" s="124" t="e">
+      <c r="I48" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J48" s="124" t="e">
+      <c r="J48" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8334,7 +8361,7 @@
       <c r="A49" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="123"/>
+      <c r="B49" s="111"/>
       <c r="C49" s="26" t="s">
         <v>34</v>
       </c>
@@ -8346,20 +8373,20 @@
         <f>SUM(E50:E54)</f>
         <v>0</v>
       </c>
-      <c r="F49" s="126" t="e">
+      <c r="F49" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G49" s="129"/>
+      <c r="G49" s="96"/>
       <c r="H49" s="30">
         <f>SUM(H50:H54)</f>
         <v>0</v>
       </c>
-      <c r="I49" s="124" t="e">
+      <c r="I49" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J49" s="124" t="e">
+      <c r="J49" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8369,23 +8396,23 @@
       <c r="A50" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="123"/>
+      <c r="B50" s="111"/>
       <c r="C50" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="30"/>
-      <c r="F50" s="126" t="e">
+      <c r="F50" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G50" s="129"/>
+      <c r="G50" s="96"/>
       <c r="H50" s="30"/>
-      <c r="I50" s="124" t="e">
+      <c r="I50" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J50" s="124" t="e">
+      <c r="J50" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8395,23 +8422,23 @@
       <c r="A51" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="123"/>
+      <c r="B51" s="111"/>
       <c r="C51" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D51" s="30"/>
       <c r="E51" s="30"/>
-      <c r="F51" s="126" t="e">
+      <c r="F51" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G51" s="129"/>
+      <c r="G51" s="96"/>
       <c r="H51" s="30"/>
-      <c r="I51" s="124" t="e">
+      <c r="I51" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J51" s="124" t="e">
+      <c r="J51" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8421,23 +8448,23 @@
       <c r="A52" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="123"/>
+      <c r="B52" s="111"/>
       <c r="C52" s="38" t="s">
         <v>96</v>
       </c>
       <c r="D52" s="30"/>
       <c r="E52" s="30"/>
-      <c r="F52" s="126" t="e">
+      <c r="F52" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G52" s="129"/>
+      <c r="G52" s="96"/>
       <c r="H52" s="30"/>
-      <c r="I52" s="124" t="e">
+      <c r="I52" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J52" s="124" t="e">
+      <c r="J52" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8447,23 +8474,23 @@
       <c r="A53" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B53" s="123"/>
+      <c r="B53" s="111"/>
       <c r="C53" s="38" t="s">
         <v>70</v>
       </c>
       <c r="D53" s="30"/>
       <c r="E53" s="30"/>
-      <c r="F53" s="126" t="e">
+      <c r="F53" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G53" s="129"/>
+      <c r="G53" s="96"/>
       <c r="H53" s="30"/>
-      <c r="I53" s="124" t="e">
+      <c r="I53" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J53" s="124" t="e">
+      <c r="J53" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8473,23 +8500,23 @@
       <c r="A54" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="123"/>
+      <c r="B54" s="111"/>
       <c r="C54" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D54" s="30"/>
       <c r="E54" s="30"/>
-      <c r="F54" s="126" t="e">
+      <c r="F54" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G54" s="129"/>
+      <c r="G54" s="96"/>
       <c r="H54" s="30"/>
-      <c r="I54" s="124" t="e">
+      <c r="I54" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J54" s="124" t="e">
+      <c r="J54" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8499,7 +8526,7 @@
       <c r="A55" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B55" s="123"/>
+      <c r="B55" s="111"/>
       <c r="C55" s="26" t="s">
         <v>36</v>
       </c>
@@ -8511,20 +8538,20 @@
         <f>SUM(E56:E60)</f>
         <v>0</v>
       </c>
-      <c r="F55" s="126" t="e">
+      <c r="F55" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G55" s="129"/>
+      <c r="G55" s="96"/>
       <c r="H55" s="30">
         <f>SUM(H56:H60)</f>
         <v>0</v>
       </c>
-      <c r="I55" s="124" t="e">
+      <c r="I55" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J55" s="124" t="e">
+      <c r="J55" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8534,23 +8561,23 @@
       <c r="A56" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B56" s="123"/>
+      <c r="B56" s="111"/>
       <c r="C56" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D56" s="30"/>
       <c r="E56" s="30"/>
-      <c r="F56" s="126" t="e">
+      <c r="F56" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G56" s="129"/>
+      <c r="G56" s="96"/>
       <c r="H56" s="21"/>
-      <c r="I56" s="124" t="e">
+      <c r="I56" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J56" s="124" t="e">
+      <c r="J56" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8560,23 +8587,23 @@
       <c r="A57" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="123"/>
+      <c r="B57" s="111"/>
       <c r="C57" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D57" s="30"/>
       <c r="E57" s="30"/>
-      <c r="F57" s="126" t="e">
+      <c r="F57" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G57" s="129"/>
+      <c r="G57" s="96"/>
       <c r="H57" s="21"/>
-      <c r="I57" s="124" t="e">
+      <c r="I57" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J57" s="124" t="e">
+      <c r="J57" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8586,23 +8613,23 @@
       <c r="A58" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B58" s="123"/>
+      <c r="B58" s="111"/>
       <c r="C58" s="38" t="s">
         <v>68</v>
       </c>
       <c r="D58" s="30"/>
       <c r="E58" s="30"/>
-      <c r="F58" s="126" t="e">
+      <c r="F58" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G58" s="129"/>
+      <c r="G58" s="96"/>
       <c r="H58" s="21"/>
-      <c r="I58" s="124" t="e">
+      <c r="I58" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J58" s="124" t="e">
+      <c r="J58" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8612,23 +8639,23 @@
       <c r="A59" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B59" s="123"/>
+      <c r="B59" s="111"/>
       <c r="C59" s="38" t="s">
         <v>70</v>
       </c>
       <c r="D59" s="30"/>
       <c r="E59" s="30"/>
-      <c r="F59" s="126" t="e">
+      <c r="F59" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G59" s="129"/>
+      <c r="G59" s="96"/>
       <c r="H59" s="21"/>
-      <c r="I59" s="124" t="e">
+      <c r="I59" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J59" s="124" t="e">
+      <c r="J59" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8638,23 +8665,23 @@
       <c r="A60" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B60" s="123"/>
+      <c r="B60" s="111"/>
       <c r="C60" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30"/>
-      <c r="F60" s="126" t="e">
+      <c r="F60" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G60" s="129"/>
+      <c r="G60" s="96"/>
       <c r="H60" s="21"/>
-      <c r="I60" s="124" t="e">
+      <c r="I60" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J60" s="124" t="e">
+      <c r="J60" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8664,7 +8691,7 @@
       <c r="A61" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="123"/>
+      <c r="B61" s="111"/>
       <c r="C61" s="32" t="s">
         <v>38</v>
       </c>
@@ -8676,20 +8703,20 @@
         <f>SUM(E62:E66)</f>
         <v>0</v>
       </c>
-      <c r="F61" s="126" t="e">
+      <c r="F61" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G61" s="129"/>
+      <c r="G61" s="96"/>
       <c r="H61" s="30">
         <f>SUM(H62:H66)</f>
         <v>0</v>
       </c>
-      <c r="I61" s="124" t="e">
+      <c r="I61" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J61" s="124" t="e">
+      <c r="J61" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8699,23 +8726,23 @@
       <c r="A62" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B62" s="123"/>
+      <c r="B62" s="111"/>
       <c r="C62" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D62" s="30"/>
       <c r="E62" s="30"/>
-      <c r="F62" s="126" t="e">
+      <c r="F62" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G62" s="129"/>
+      <c r="G62" s="96"/>
       <c r="H62" s="21"/>
-      <c r="I62" s="124" t="e">
+      <c r="I62" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J62" s="124" t="e">
+      <c r="J62" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8725,23 +8752,23 @@
       <c r="A63" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B63" s="123"/>
+      <c r="B63" s="111"/>
       <c r="C63" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D63" s="30"/>
       <c r="E63" s="30"/>
-      <c r="F63" s="126" t="e">
+      <c r="F63" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G63" s="129"/>
+      <c r="G63" s="96"/>
       <c r="H63" s="21"/>
-      <c r="I63" s="124" t="e">
+      <c r="I63" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J63" s="124" t="e">
+      <c r="J63" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8751,23 +8778,23 @@
       <c r="A64" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B64" s="123"/>
+      <c r="B64" s="111"/>
       <c r="C64" s="38" t="s">
         <v>68</v>
       </c>
       <c r="D64" s="30"/>
       <c r="E64" s="30"/>
-      <c r="F64" s="126" t="e">
+      <c r="F64" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G64" s="129"/>
+      <c r="G64" s="96"/>
       <c r="H64" s="21"/>
-      <c r="I64" s="124" t="e">
+      <c r="I64" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J64" s="124" t="e">
+      <c r="J64" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8777,23 +8804,23 @@
       <c r="A65" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B65" s="123"/>
+      <c r="B65" s="111"/>
       <c r="C65" s="38" t="s">
         <v>70</v>
       </c>
       <c r="D65" s="30"/>
       <c r="E65" s="30"/>
-      <c r="F65" s="126" t="e">
+      <c r="F65" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G65" s="129"/>
+      <c r="G65" s="96"/>
       <c r="H65" s="21"/>
-      <c r="I65" s="124" t="e">
+      <c r="I65" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J65" s="124" t="e">
+      <c r="J65" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8809,23 +8836,23 @@
       <c r="A66" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="123"/>
+      <c r="B66" s="111"/>
       <c r="C66" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D66" s="132"/>
-      <c r="E66" s="132"/>
-      <c r="F66" s="126" t="e">
+      <c r="D66" s="99"/>
+      <c r="E66" s="99"/>
+      <c r="F66" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G66" s="129"/>
-      <c r="H66" s="132"/>
-      <c r="I66" s="124" t="e">
+      <c r="G66" s="96"/>
+      <c r="H66" s="99"/>
+      <c r="I66" s="91" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J66" s="124" t="e">
+      <c r="J66" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8841,10 +8868,10 @@
       <c r="A67" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="B67" s="116" t="s">
+      <c r="B67" s="104" t="s">
         <v>112</v>
       </c>
-      <c r="C67" s="117"/>
+      <c r="C67" s="105"/>
       <c r="D67" s="30">
         <f>D61+D55+D23</f>
         <v>0</v>
@@ -8853,20 +8880,20 @@
         <f>E61+E55+E23</f>
         <v>0</v>
       </c>
-      <c r="F67" s="126" t="e">
+      <c r="F67" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G67" s="133"/>
+      <c r="G67" s="100"/>
       <c r="H67" s="30">
         <f>H61+H55+H23</f>
         <v>0</v>
       </c>
-      <c r="I67" s="134" t="e">
+      <c r="I67" s="101" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J67" s="124" t="e">
+      <c r="J67" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8882,23 +8909,23 @@
       <c r="A68" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B68" s="116" t="s">
+      <c r="B68" s="104" t="s">
         <v>114</v>
       </c>
-      <c r="C68" s="117"/>
+      <c r="C68" s="105"/>
       <c r="D68" s="30"/>
       <c r="E68" s="30"/>
-      <c r="F68" s="126" t="e">
+      <c r="F68" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G68" s="133"/>
+      <c r="G68" s="100"/>
       <c r="H68" s="30"/>
-      <c r="I68" s="134" t="e">
+      <c r="I68" s="101" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J68" s="124" t="e">
+      <c r="J68" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8914,10 +8941,10 @@
       <c r="A69" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B69" s="116" t="s">
+      <c r="B69" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="C69" s="117"/>
+      <c r="C69" s="105"/>
       <c r="D69" s="30">
         <f>$D$25+$D$31+$D$37+$D$43+$D$49</f>
         <v>0</v>
@@ -8926,20 +8953,20 @@
         <f>$E$25+$E$31+$E$37+$E$43+$E$49</f>
         <v>0</v>
       </c>
-      <c r="F69" s="126" t="e">
+      <c r="F69" s="93" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G69" s="133"/>
+      <c r="G69" s="100"/>
       <c r="H69" s="30">
         <f>$H$25+$H$31+$H$37+$H$43+$H$49</f>
         <v>0</v>
       </c>
-      <c r="I69" s="134" t="e">
+      <c r="I69" s="101" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J69" s="124" t="e">
+      <c r="J69" s="91" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -8955,17 +8982,17 @@
       <c r="A70" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B70" s="116" t="s">
+      <c r="B70" s="104" t="s">
         <v>118</v>
       </c>
-      <c r="C70" s="117"/>
-      <c r="D70" s="118"/>
-      <c r="E70" s="119"/>
-      <c r="F70" s="119"/>
-      <c r="G70" s="119"/>
-      <c r="H70" s="119"/>
-      <c r="I70" s="119"/>
-      <c r="J70" s="120"/>
+      <c r="C70" s="105"/>
+      <c r="D70" s="137"/>
+      <c r="E70" s="138"/>
+      <c r="F70" s="138"/>
+      <c r="G70" s="138"/>
+      <c r="H70" s="138"/>
+      <c r="I70" s="138"/>
+      <c r="J70" s="139"/>
       <c r="K70" s="18"/>
       <c r="L70" s="45"/>
       <c r="M70" s="42"/>
@@ -8978,17 +9005,17 @@
       <c r="A71" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B71" s="116" t="s">
+      <c r="B71" s="104" t="s">
         <v>120</v>
       </c>
-      <c r="C71" s="117"/>
-      <c r="D71" s="118"/>
-      <c r="E71" s="119"/>
-      <c r="F71" s="119"/>
-      <c r="G71" s="119"/>
-      <c r="H71" s="119"/>
-      <c r="I71" s="119"/>
-      <c r="J71" s="120"/>
+      <c r="C71" s="105"/>
+      <c r="D71" s="137"/>
+      <c r="E71" s="138"/>
+      <c r="F71" s="138"/>
+      <c r="G71" s="138"/>
+      <c r="H71" s="138"/>
+      <c r="I71" s="138"/>
+      <c r="J71" s="139"/>
       <c r="K71" s="18"/>
       <c r="L71" s="46"/>
       <c r="M71" s="44"/>
@@ -9001,20 +9028,20 @@
       <c r="A72" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="B72" s="116" t="s">
+      <c r="B72" s="104" t="s">
         <v>122</v>
       </c>
-      <c r="C72" s="117"/>
-      <c r="D72" s="118" t="e">
+      <c r="C72" s="105"/>
+      <c r="D72" s="106" t="e">
         <f>D70/H67</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E72" s="119"/>
-      <c r="F72" s="119"/>
-      <c r="G72" s="119"/>
-      <c r="H72" s="119"/>
-      <c r="I72" s="119"/>
-      <c r="J72" s="120"/>
+      <c r="E72" s="107"/>
+      <c r="F72" s="107"/>
+      <c r="G72" s="107"/>
+      <c r="H72" s="107"/>
+      <c r="I72" s="107"/>
+      <c r="J72" s="108"/>
       <c r="K72" s="18"/>
       <c r="L72" s="44"/>
       <c r="M72" s="42"/>
@@ -9027,20 +9054,20 @@
       <c r="A73" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B73" s="116" t="s">
+      <c r="B73" s="104" t="s">
         <v>124</v>
       </c>
-      <c r="C73" s="117"/>
-      <c r="D73" s="118" t="e">
+      <c r="C73" s="105"/>
+      <c r="D73" s="106" t="e">
         <f>D71/H67</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E73" s="119"/>
-      <c r="F73" s="119"/>
-      <c r="G73" s="119"/>
-      <c r="H73" s="119"/>
-      <c r="I73" s="119"/>
-      <c r="J73" s="120"/>
+      <c r="E73" s="107"/>
+      <c r="F73" s="107"/>
+      <c r="G73" s="107"/>
+      <c r="H73" s="107"/>
+      <c r="I73" s="107"/>
+      <c r="J73" s="108"/>
       <c r="K73" s="18"/>
       <c r="L73" s="42"/>
       <c r="M73" s="42"/>
@@ -9053,20 +9080,20 @@
       <c r="A74" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B74" s="116" t="s">
+      <c r="B74" s="104" t="s">
         <v>126</v>
       </c>
-      <c r="C74" s="117"/>
-      <c r="D74" s="118" t="e">
+      <c r="C74" s="105"/>
+      <c r="D74" s="106" t="e">
         <f>(D70+D71)/H67</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E74" s="119"/>
-      <c r="F74" s="119"/>
-      <c r="G74" s="119"/>
-      <c r="H74" s="119"/>
-      <c r="I74" s="119"/>
-      <c r="J74" s="120"/>
+      <c r="E74" s="107"/>
+      <c r="F74" s="107"/>
+      <c r="G74" s="107"/>
+      <c r="H74" s="107"/>
+      <c r="I74" s="107"/>
+      <c r="J74" s="108"/>
       <c r="K74" s="18"/>
       <c r="L74" s="42"/>
       <c r="M74" s="7"/>
@@ -9079,20 +9106,20 @@
       <c r="A75" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B75" s="116" t="s">
+      <c r="B75" s="104" t="s">
         <v>128</v>
       </c>
-      <c r="C75" s="117"/>
-      <c r="D75" s="118" t="e">
+      <c r="C75" s="105"/>
+      <c r="D75" s="106" t="e">
         <f>D70/H69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E75" s="119"/>
-      <c r="F75" s="119"/>
-      <c r="G75" s="119"/>
-      <c r="H75" s="119"/>
-      <c r="I75" s="119"/>
-      <c r="J75" s="120"/>
+      <c r="E75" s="107"/>
+      <c r="F75" s="107"/>
+      <c r="G75" s="107"/>
+      <c r="H75" s="107"/>
+      <c r="I75" s="107"/>
+      <c r="J75" s="108"/>
       <c r="K75" s="18"/>
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
@@ -9105,20 +9132,20 @@
       <c r="A76" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B76" s="116" t="s">
+      <c r="B76" s="104" t="s">
         <v>130</v>
       </c>
-      <c r="C76" s="117"/>
-      <c r="D76" s="118" t="e">
+      <c r="C76" s="105"/>
+      <c r="D76" s="106" t="e">
         <f>D71/H69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E76" s="119"/>
-      <c r="F76" s="119"/>
-      <c r="G76" s="119"/>
-      <c r="H76" s="119"/>
-      <c r="I76" s="119"/>
-      <c r="J76" s="120"/>
+      <c r="E76" s="107"/>
+      <c r="F76" s="107"/>
+      <c r="G76" s="107"/>
+      <c r="H76" s="107"/>
+      <c r="I76" s="107"/>
+      <c r="J76" s="108"/>
       <c r="K76" s="18"/>
       <c r="L76" s="7"/>
       <c r="M76" s="7"/>
@@ -9131,20 +9158,20 @@
       <c r="A77" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B77" s="116" t="s">
+      <c r="B77" s="104" t="s">
         <v>132</v>
       </c>
-      <c r="C77" s="117"/>
-      <c r="D77" s="118" t="e">
+      <c r="C77" s="105"/>
+      <c r="D77" s="106" t="e">
         <f>(F70+F71)/H69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E77" s="119"/>
-      <c r="F77" s="119"/>
-      <c r="G77" s="119"/>
-      <c r="H77" s="119"/>
-      <c r="I77" s="119"/>
-      <c r="J77" s="120"/>
+      <c r="E77" s="107"/>
+      <c r="F77" s="107"/>
+      <c r="G77" s="107"/>
+      <c r="H77" s="107"/>
+      <c r="I77" s="107"/>
+      <c r="J77" s="108"/>
       <c r="K77" s="18"/>
       <c r="L77" s="7"/>
       <c r="M77" s="7"/>
@@ -9227,7 +9254,7 @@
       <c r="J82" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="K82" s="136" t="s">
+      <c r="K82" s="103" t="s">
         <v>148</v>
       </c>
       <c r="L82" s="58"/>
@@ -9459,7 +9486,7 @@
         <v>0</v>
       </c>
       <c r="D88" s="73">
-        <f t="shared" ref="D88:J88" si="5">SUM(D83:D87)</f>
+        <f t="shared" ref="D88:I88" si="5">SUM(D83:D87)</f>
         <v>0</v>
       </c>
       <c r="E88" s="73">
@@ -9482,7 +9509,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J88" s="135">
+      <c r="J88" s="102">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -9586,14 +9613,18 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="D77:J77"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:J74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:J75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:J76"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="D73:J73"/>
     <mergeCell ref="B23:B24"/>
@@ -9607,18 +9638,14 @@
     <mergeCell ref="D71:J71"/>
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="D72:J72"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:C5"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="D77:J77"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:J74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:J75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:J76"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Auto-committed on 2022/03/08 週二
</commit_message>
<xml_diff>
--- a/Program/Other/LY003_底稿_非RBC_表14-2_會計部年度檢查報表.xlsx
+++ b/Program/Other/LY003_底稿_非RBC_表14-2_會計部年度檢查報表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3821,6 +3821,83 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3847,83 +3924,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="13" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -6981,8 +6981,8 @@
   </sheetPr>
   <dimension ref="A1:Y116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71:J71"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
@@ -7022,11 +7022,11 @@
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -7040,39 +7040,39 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:13" s="7" customFormat="1">
-      <c r="A3" s="127" t="s">
+      <c r="A3" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="130"/>
-      <c r="D3" s="135" t="s">
+      <c r="C3" s="111"/>
+      <c r="D3" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="136"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="123" t="s">
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="112" t="s">
+      <c r="H3" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="112" t="s">
+      <c r="I3" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="114" t="s">
+      <c r="J3" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="116" t="s">
+      <c r="K3" s="122" t="s">
         <v>10</v>
       </c>
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:13" s="7" customFormat="1">
-      <c r="A4" s="128"/>
-      <c r="B4" s="131"/>
-      <c r="C4" s="132"/>
+      <c r="A4" s="109"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="113"/>
       <c r="D4" s="10" t="s">
         <v>11</v>
       </c>
@@ -7082,17 +7082,17 @@
       <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="124"/>
-      <c r="H4" s="113"/>
-      <c r="I4" s="113"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="117"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
+      <c r="J4" s="121"/>
+      <c r="K4" s="123"/>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:13" s="7" customFormat="1">
-      <c r="A5" s="128"/>
-      <c r="B5" s="133"/>
-      <c r="C5" s="134"/>
+      <c r="A5" s="109"/>
+      <c r="B5" s="114"/>
+      <c r="C5" s="115"/>
       <c r="D5" s="12" t="s">
         <v>14</v>
       </c>
@@ -7124,7 +7124,7 @@
       <c r="A6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="118" t="s">
+      <c r="B6" s="124" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -7158,7 +7158,7 @@
       <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="119"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="17" t="s">
         <v>27</v>
       </c>
@@ -7196,7 +7196,7 @@
       <c r="A8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="120"/>
+      <c r="B8" s="105"/>
       <c r="C8" s="26" t="s">
         <v>30</v>
       </c>
@@ -7226,7 +7226,7 @@
       <c r="A9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="120"/>
+      <c r="B9" s="105"/>
       <c r="C9" s="26" t="s">
         <v>32</v>
       </c>
@@ -7253,7 +7253,7 @@
       <c r="A10" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="120"/>
+      <c r="B10" s="105"/>
       <c r="C10" s="26" t="s">
         <v>34</v>
       </c>
@@ -7280,7 +7280,7 @@
       <c r="A11" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="120"/>
+      <c r="B11" s="105"/>
       <c r="C11" s="26" t="s">
         <v>36</v>
       </c>
@@ -7307,7 +7307,7 @@
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="120"/>
+      <c r="B12" s="105"/>
       <c r="C12" s="32" t="s">
         <v>38</v>
       </c>
@@ -7334,7 +7334,7 @@
       <c r="A13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="120"/>
+      <c r="B13" s="105"/>
       <c r="C13" s="32" t="s">
         <v>40</v>
       </c>
@@ -7370,7 +7370,7 @@
       <c r="A14" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="121" t="s">
+      <c r="B14" s="104" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="26" t="s">
@@ -7399,7 +7399,7 @@
       <c r="A15" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="120"/>
+      <c r="B15" s="105"/>
       <c r="C15" s="26" t="s">
         <v>45</v>
       </c>
@@ -7426,7 +7426,7 @@
       <c r="A16" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="120"/>
+      <c r="B16" s="105"/>
       <c r="C16" s="26" t="s">
         <v>47</v>
       </c>
@@ -7453,7 +7453,7 @@
       <c r="A17" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="122"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="37" t="s">
         <v>49</v>
       </c>
@@ -7479,7 +7479,7 @@
       <c r="A18" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="122"/>
+      <c r="B18" s="126"/>
       <c r="C18" s="37" t="s">
         <v>40</v>
       </c>
@@ -7514,7 +7514,7 @@
       <c r="A19" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="104" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="26" t="s">
@@ -7542,7 +7542,7 @@
       <c r="A20" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="120"/>
+      <c r="B20" s="105"/>
       <c r="C20" s="26" t="s">
         <v>45</v>
       </c>
@@ -7568,7 +7568,7 @@
       <c r="A21" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="120"/>
+      <c r="B21" s="105"/>
       <c r="C21" s="26" t="s">
         <v>47</v>
       </c>
@@ -7594,7 +7594,7 @@
       <c r="A22" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="120"/>
+      <c r="B22" s="105"/>
       <c r="C22" s="37" t="s">
         <v>49</v>
       </c>
@@ -7620,7 +7620,7 @@
       <c r="A23" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="109" t="s">
+      <c r="B23" s="134" t="s">
         <v>57</v>
       </c>
       <c r="C23" s="37" t="s">
@@ -7657,7 +7657,7 @@
       <c r="A24" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="110"/>
+      <c r="B24" s="135"/>
       <c r="C24" s="37" t="s">
         <v>60</v>
       </c>
@@ -7683,7 +7683,7 @@
       <c r="A25" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="109" t="s">
+      <c r="B25" s="134" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="26" t="s">
@@ -7720,7 +7720,7 @@
       <c r="A26" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="111"/>
+      <c r="B26" s="136"/>
       <c r="C26" s="38" t="s">
         <v>64</v>
       </c>
@@ -7746,7 +7746,7 @@
       <c r="A27" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="111"/>
+      <c r="B27" s="136"/>
       <c r="C27" s="38" t="s">
         <v>66</v>
       </c>
@@ -7772,7 +7772,7 @@
       <c r="A28" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="111"/>
+      <c r="B28" s="136"/>
       <c r="C28" s="38" t="s">
         <v>68</v>
       </c>
@@ -7798,7 +7798,7 @@
       <c r="A29" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="111"/>
+      <c r="B29" s="136"/>
       <c r="C29" s="38" t="s">
         <v>70</v>
       </c>
@@ -7824,7 +7824,7 @@
       <c r="A30" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="111"/>
+      <c r="B30" s="136"/>
       <c r="C30" s="38" t="s">
         <v>72</v>
       </c>
@@ -7850,7 +7850,7 @@
       <c r="A31" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="111"/>
+      <c r="B31" s="136"/>
       <c r="C31" s="26" t="s">
         <v>27</v>
       </c>
@@ -7885,7 +7885,7 @@
       <c r="A32" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="111"/>
+      <c r="B32" s="136"/>
       <c r="C32" s="38" t="s">
         <v>64</v>
       </c>
@@ -7911,7 +7911,7 @@
       <c r="A33" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="111"/>
+      <c r="B33" s="136"/>
       <c r="C33" s="38" t="s">
         <v>66</v>
       </c>
@@ -7938,7 +7938,7 @@
       <c r="A34" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="111"/>
+      <c r="B34" s="136"/>
       <c r="C34" s="38" t="s">
         <v>68</v>
       </c>
@@ -7965,7 +7965,7 @@
       <c r="A35" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="111"/>
+      <c r="B35" s="136"/>
       <c r="C35" s="38" t="s">
         <v>70</v>
       </c>
@@ -7992,7 +7992,7 @@
       <c r="A36" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="111"/>
+      <c r="B36" s="136"/>
       <c r="C36" s="38" t="s">
         <v>72</v>
       </c>
@@ -8019,7 +8019,7 @@
       <c r="A37" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="111"/>
+      <c r="B37" s="136"/>
       <c r="C37" s="26" t="s">
         <v>30</v>
       </c>
@@ -8055,7 +8055,7 @@
       <c r="A38" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="111"/>
+      <c r="B38" s="136"/>
       <c r="C38" s="38" t="s">
         <v>64</v>
       </c>
@@ -8082,7 +8082,7 @@
       <c r="A39" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="111"/>
+      <c r="B39" s="136"/>
       <c r="C39" s="38" t="s">
         <v>66</v>
       </c>
@@ -8109,7 +8109,7 @@
       <c r="A40" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="111"/>
+      <c r="B40" s="136"/>
       <c r="C40" s="38" t="s">
         <v>68</v>
       </c>
@@ -8136,7 +8136,7 @@
       <c r="A41" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="111"/>
+      <c r="B41" s="136"/>
       <c r="C41" s="38" t="s">
         <v>70</v>
       </c>
@@ -8163,7 +8163,7 @@
       <c r="A42" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="111"/>
+      <c r="B42" s="136"/>
       <c r="C42" s="38" t="s">
         <v>72</v>
       </c>
@@ -8190,7 +8190,7 @@
       <c r="A43" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="111"/>
+      <c r="B43" s="136"/>
       <c r="C43" s="26" t="s">
         <v>86</v>
       </c>
@@ -8226,7 +8226,7 @@
       <c r="A44" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="111"/>
+      <c r="B44" s="136"/>
       <c r="C44" s="38" t="s">
         <v>64</v>
       </c>
@@ -8253,7 +8253,7 @@
       <c r="A45" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="111"/>
+      <c r="B45" s="136"/>
       <c r="C45" s="38" t="s">
         <v>66</v>
       </c>
@@ -8280,7 +8280,7 @@
       <c r="A46" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="111"/>
+      <c r="B46" s="136"/>
       <c r="C46" s="38" t="s">
         <v>68</v>
       </c>
@@ -8307,7 +8307,7 @@
       <c r="A47" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="111"/>
+      <c r="B47" s="136"/>
       <c r="C47" s="38" t="s">
         <v>70</v>
       </c>
@@ -8334,7 +8334,7 @@
       <c r="A48" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="111"/>
+      <c r="B48" s="136"/>
       <c r="C48" s="38" t="s">
         <v>72</v>
       </c>
@@ -8361,7 +8361,7 @@
       <c r="A49" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="111"/>
+      <c r="B49" s="136"/>
       <c r="C49" s="26" t="s">
         <v>34</v>
       </c>
@@ -8396,7 +8396,7 @@
       <c r="A50" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="111"/>
+      <c r="B50" s="136"/>
       <c r="C50" s="38" t="s">
         <v>64</v>
       </c>
@@ -8422,7 +8422,7 @@
       <c r="A51" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="111"/>
+      <c r="B51" s="136"/>
       <c r="C51" s="38" t="s">
         <v>66</v>
       </c>
@@ -8448,7 +8448,7 @@
       <c r="A52" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="111"/>
+      <c r="B52" s="136"/>
       <c r="C52" s="38" t="s">
         <v>96</v>
       </c>
@@ -8474,7 +8474,7 @@
       <c r="A53" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B53" s="111"/>
+      <c r="B53" s="136"/>
       <c r="C53" s="38" t="s">
         <v>70</v>
       </c>
@@ -8500,7 +8500,7 @@
       <c r="A54" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="111"/>
+      <c r="B54" s="136"/>
       <c r="C54" s="38" t="s">
         <v>72</v>
       </c>
@@ -8526,7 +8526,7 @@
       <c r="A55" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B55" s="111"/>
+      <c r="B55" s="136"/>
       <c r="C55" s="26" t="s">
         <v>36</v>
       </c>
@@ -8561,7 +8561,7 @@
       <c r="A56" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B56" s="111"/>
+      <c r="B56" s="136"/>
       <c r="C56" s="38" t="s">
         <v>64</v>
       </c>
@@ -8587,7 +8587,7 @@
       <c r="A57" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="111"/>
+      <c r="B57" s="136"/>
       <c r="C57" s="38" t="s">
         <v>66</v>
       </c>
@@ -8613,7 +8613,7 @@
       <c r="A58" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B58" s="111"/>
+      <c r="B58" s="136"/>
       <c r="C58" s="38" t="s">
         <v>68</v>
       </c>
@@ -8639,7 +8639,7 @@
       <c r="A59" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B59" s="111"/>
+      <c r="B59" s="136"/>
       <c r="C59" s="38" t="s">
         <v>70</v>
       </c>
@@ -8665,7 +8665,7 @@
       <c r="A60" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B60" s="111"/>
+      <c r="B60" s="136"/>
       <c r="C60" s="38" t="s">
         <v>72</v>
       </c>
@@ -8691,7 +8691,7 @@
       <c r="A61" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="111"/>
+      <c r="B61" s="136"/>
       <c r="C61" s="32" t="s">
         <v>38</v>
       </c>
@@ -8726,7 +8726,7 @@
       <c r="A62" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B62" s="111"/>
+      <c r="B62" s="136"/>
       <c r="C62" s="38" t="s">
         <v>64</v>
       </c>
@@ -8752,7 +8752,7 @@
       <c r="A63" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B63" s="111"/>
+      <c r="B63" s="136"/>
       <c r="C63" s="38" t="s">
         <v>66</v>
       </c>
@@ -8778,7 +8778,7 @@
       <c r="A64" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B64" s="111"/>
+      <c r="B64" s="136"/>
       <c r="C64" s="38" t="s">
         <v>68</v>
       </c>
@@ -8804,7 +8804,7 @@
       <c r="A65" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B65" s="111"/>
+      <c r="B65" s="136"/>
       <c r="C65" s="38" t="s">
         <v>70</v>
       </c>
@@ -8836,7 +8836,7 @@
       <c r="A66" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="111"/>
+      <c r="B66" s="136"/>
       <c r="C66" s="38" t="s">
         <v>72</v>
       </c>
@@ -8868,10 +8868,10 @@
       <c r="A67" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="B67" s="104" t="s">
+      <c r="B67" s="129" t="s">
         <v>112</v>
       </c>
-      <c r="C67" s="105"/>
+      <c r="C67" s="130"/>
       <c r="D67" s="30">
         <f>D61+D55+D23</f>
         <v>0</v>
@@ -8909,10 +8909,10 @@
       <c r="A68" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B68" s="104" t="s">
+      <c r="B68" s="129" t="s">
         <v>114</v>
       </c>
-      <c r="C68" s="105"/>
+      <c r="C68" s="130"/>
       <c r="D68" s="30"/>
       <c r="E68" s="30"/>
       <c r="F68" s="93" t="e">
@@ -8941,10 +8941,10 @@
       <c r="A69" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B69" s="104" t="s">
+      <c r="B69" s="129" t="s">
         <v>116</v>
       </c>
-      <c r="C69" s="105"/>
+      <c r="C69" s="130"/>
       <c r="D69" s="30">
         <f>$D$25+$D$31+$D$37+$D$43+$D$49</f>
         <v>0</v>
@@ -8982,10 +8982,10 @@
       <c r="A70" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B70" s="104" t="s">
+      <c r="B70" s="129" t="s">
         <v>118</v>
       </c>
-      <c r="C70" s="105"/>
+      <c r="C70" s="130"/>
       <c r="D70" s="137"/>
       <c r="E70" s="138"/>
       <c r="F70" s="138"/>
@@ -9005,10 +9005,10 @@
       <c r="A71" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B71" s="104" t="s">
+      <c r="B71" s="129" t="s">
         <v>120</v>
       </c>
-      <c r="C71" s="105"/>
+      <c r="C71" s="130"/>
       <c r="D71" s="137"/>
       <c r="E71" s="138"/>
       <c r="F71" s="138"/>
@@ -9028,20 +9028,20 @@
       <c r="A72" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="B72" s="104" t="s">
+      <c r="B72" s="129" t="s">
         <v>122</v>
       </c>
-      <c r="C72" s="105"/>
-      <c r="D72" s="106" t="e">
+      <c r="C72" s="130"/>
+      <c r="D72" s="131" t="e">
         <f>D70/H67</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E72" s="107"/>
-      <c r="F72" s="107"/>
-      <c r="G72" s="107"/>
-      <c r="H72" s="107"/>
-      <c r="I72" s="107"/>
-      <c r="J72" s="108"/>
+      <c r="E72" s="132"/>
+      <c r="F72" s="132"/>
+      <c r="G72" s="132"/>
+      <c r="H72" s="132"/>
+      <c r="I72" s="132"/>
+      <c r="J72" s="133"/>
       <c r="K72" s="18"/>
       <c r="L72" s="44"/>
       <c r="M72" s="42"/>
@@ -9054,20 +9054,20 @@
       <c r="A73" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B73" s="104" t="s">
+      <c r="B73" s="129" t="s">
         <v>124</v>
       </c>
-      <c r="C73" s="105"/>
-      <c r="D73" s="106" t="e">
+      <c r="C73" s="130"/>
+      <c r="D73" s="131" t="e">
         <f>D71/H67</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E73" s="107"/>
-      <c r="F73" s="107"/>
-      <c r="G73" s="107"/>
-      <c r="H73" s="107"/>
-      <c r="I73" s="107"/>
-      <c r="J73" s="108"/>
+      <c r="E73" s="132"/>
+      <c r="F73" s="132"/>
+      <c r="G73" s="132"/>
+      <c r="H73" s="132"/>
+      <c r="I73" s="132"/>
+      <c r="J73" s="133"/>
       <c r="K73" s="18"/>
       <c r="L73" s="42"/>
       <c r="M73" s="42"/>
@@ -9080,20 +9080,20 @@
       <c r="A74" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B74" s="104" t="s">
+      <c r="B74" s="129" t="s">
         <v>126</v>
       </c>
-      <c r="C74" s="105"/>
-      <c r="D74" s="106" t="e">
+      <c r="C74" s="130"/>
+      <c r="D74" s="131" t="e">
         <f>(D70+D71)/H67</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E74" s="107"/>
-      <c r="F74" s="107"/>
-      <c r="G74" s="107"/>
-      <c r="H74" s="107"/>
-      <c r="I74" s="107"/>
-      <c r="J74" s="108"/>
+      <c r="E74" s="132"/>
+      <c r="F74" s="132"/>
+      <c r="G74" s="132"/>
+      <c r="H74" s="132"/>
+      <c r="I74" s="132"/>
+      <c r="J74" s="133"/>
       <c r="K74" s="18"/>
       <c r="L74" s="42"/>
       <c r="M74" s="7"/>
@@ -9106,20 +9106,20 @@
       <c r="A75" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B75" s="104" t="s">
+      <c r="B75" s="129" t="s">
         <v>128</v>
       </c>
-      <c r="C75" s="105"/>
-      <c r="D75" s="106" t="e">
+      <c r="C75" s="130"/>
+      <c r="D75" s="131" t="e">
         <f>D70/H69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E75" s="107"/>
-      <c r="F75" s="107"/>
-      <c r="G75" s="107"/>
-      <c r="H75" s="107"/>
-      <c r="I75" s="107"/>
-      <c r="J75" s="108"/>
+      <c r="E75" s="132"/>
+      <c r="F75" s="132"/>
+      <c r="G75" s="132"/>
+      <c r="H75" s="132"/>
+      <c r="I75" s="132"/>
+      <c r="J75" s="133"/>
       <c r="K75" s="18"/>
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
@@ -9132,20 +9132,20 @@
       <c r="A76" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B76" s="104" t="s">
+      <c r="B76" s="129" t="s">
         <v>130</v>
       </c>
-      <c r="C76" s="105"/>
-      <c r="D76" s="106" t="e">
+      <c r="C76" s="130"/>
+      <c r="D76" s="131" t="e">
         <f>D71/H69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E76" s="107"/>
-      <c r="F76" s="107"/>
-      <c r="G76" s="107"/>
-      <c r="H76" s="107"/>
-      <c r="I76" s="107"/>
-      <c r="J76" s="108"/>
+      <c r="E76" s="132"/>
+      <c r="F76" s="132"/>
+      <c r="G76" s="132"/>
+      <c r="H76" s="132"/>
+      <c r="I76" s="132"/>
+      <c r="J76" s="133"/>
       <c r="K76" s="18"/>
       <c r="L76" s="7"/>
       <c r="M76" s="7"/>
@@ -9158,20 +9158,20 @@
       <c r="A77" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B77" s="104" t="s">
+      <c r="B77" s="129" t="s">
         <v>132</v>
       </c>
-      <c r="C77" s="105"/>
-      <c r="D77" s="106" t="e">
+      <c r="C77" s="130"/>
+      <c r="D77" s="131" t="e">
         <f>(F70+F71)/H69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E77" s="107"/>
-      <c r="F77" s="107"/>
-      <c r="G77" s="107"/>
-      <c r="H77" s="107"/>
-      <c r="I77" s="107"/>
-      <c r="J77" s="108"/>
+      <c r="E77" s="132"/>
+      <c r="F77" s="132"/>
+      <c r="G77" s="132"/>
+      <c r="H77" s="132"/>
+      <c r="I77" s="132"/>
+      <c r="J77" s="133"/>
       <c r="K77" s="18"/>
       <c r="L77" s="7"/>
       <c r="M77" s="7"/>
@@ -9273,15 +9273,19 @@
         <v>0</v>
       </c>
       <c r="D83" s="61">
+        <f>H32*0.5%</f>
         <v>0</v>
       </c>
       <c r="E83" s="61">
+        <f>H38*0.5%</f>
         <v>0</v>
       </c>
       <c r="F83" s="61">
+        <f>H44*0.5%</f>
         <v>0</v>
       </c>
       <c r="G83" s="61">
+        <f>H50*0.5%</f>
         <v>0</v>
       </c>
       <c r="H83" s="62">
@@ -9316,16 +9320,20 @@
       <c r="C84" s="67">
         <v>0</v>
       </c>
-      <c r="D84" s="67">
+      <c r="D84" s="61">
+        <f>H33*2%</f>
         <v>0</v>
       </c>
       <c r="E84" s="61">
+        <f>H39*2%</f>
         <v>0</v>
       </c>
       <c r="F84" s="61">
+        <f>H45*2%</f>
         <v>0</v>
       </c>
       <c r="G84" s="61">
+        <f>H51*2%</f>
         <v>0</v>
       </c>
       <c r="H84" s="62">
@@ -9358,16 +9366,20 @@
       <c r="C85" s="67">
         <v>0</v>
       </c>
-      <c r="D85" s="67">
+      <c r="D85" s="61">
+        <f>H34*10%</f>
         <v>0</v>
       </c>
       <c r="E85" s="61">
+        <f t="shared" ref="E84:F87" si="5">H40*10%</f>
         <v>0</v>
       </c>
       <c r="F85" s="61">
+        <f>H46*10%</f>
         <v>0</v>
       </c>
       <c r="G85" s="61">
+        <f>H52*10%</f>
         <v>0</v>
       </c>
       <c r="H85" s="62">
@@ -9401,15 +9413,19 @@
         <v>0</v>
       </c>
       <c r="D86" s="61">
+        <f>H35*50%</f>
         <v>0</v>
       </c>
       <c r="E86" s="61">
+        <f>H41*50%</f>
         <v>0</v>
       </c>
       <c r="F86" s="61">
+        <f>H47*50%</f>
         <v>0</v>
       </c>
       <c r="G86" s="61">
+        <f>H53*50%</f>
         <v>0</v>
       </c>
       <c r="H86" s="62">
@@ -9443,15 +9459,19 @@
         <v>0</v>
       </c>
       <c r="D87" s="61">
+        <f>H36*100%</f>
         <v>0</v>
       </c>
       <c r="E87" s="61">
+        <f>H42*100%</f>
         <v>0</v>
       </c>
       <c r="F87" s="61">
+        <f>H48*100%</f>
         <v>0</v>
       </c>
       <c r="G87" s="61">
+        <f>H54*100%</f>
         <v>0</v>
       </c>
       <c r="H87" s="62">
@@ -9486,27 +9506,27 @@
         <v>0</v>
       </c>
       <c r="D88" s="73">
-        <f t="shared" ref="D88:I88" si="5">SUM(D83:D87)</f>
+        <f>SUM(D83:D87)</f>
         <v>0</v>
       </c>
       <c r="E88" s="73">
-        <f t="shared" si="5"/>
+        <f>SUM(E83:E87)</f>
         <v>0</v>
       </c>
       <c r="F88" s="73">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D88:I88" si="6">SUM(F83:F87)</f>
         <v>0</v>
       </c>
       <c r="G88" s="73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H88" s="73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I88" s="73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J88" s="102">
@@ -9613,18 +9633,14 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="D77:J77"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:J74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:J75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:J76"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="D73:J73"/>
     <mergeCell ref="B23:B24"/>
@@ -9638,14 +9654,18 @@
     <mergeCell ref="D71:J71"/>
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="D72:J72"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="D77:J77"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:J74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:J75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:J76"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:C5"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Auto-committed on 2022/08/03 週三 17:47:57.00
</commit_message>
<xml_diff>
--- a/Program/Other/LY003_底稿_非RBC_表14-2_會計部年度檢查報表.xlsx
+++ b/Program/Other/LY003_底稿_非RBC_表14-2_會計部年度檢查報表.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="340" windowWidth="18070" windowHeight="7320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14420" windowHeight="6110"/>
   </bookViews>
   <sheets>
     <sheet name="表14-2" sheetId="1" r:id="rId1"/>
+    <sheet name="A142放款餘額彙總表" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
@@ -23,9 +23,30 @@
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="__123Graph_X" hidden="1">'[1]5DAYRPT '!#REF!</definedName>
+    <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
+    <definedName name="_AtRisk_SimSetting_AutomaticResultsDisplayMode" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergenceConfidenceLevel" hidden="1">0.95</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergencePercentileToTest" hidden="1">0.9</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergencePerformMeanTest" hidden="1">TRUE</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergencePerformPercentileTest" hidden="1">FALSE</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergencePerformStdDeviationTest" hidden="1">FALSE</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergenceTestAllOutputs" hidden="1">TRUE</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergenceTestingPeriod" hidden="1">100</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergenceTolerance" hidden="1">0.03</definedName>
+    <definedName name="_AtRisk_SimSetting_LiveUpdate" hidden="1">TRUE</definedName>
+    <definedName name="_AtRisk_SimSetting_LiveUpdatePeriod" hidden="1">-1</definedName>
+    <definedName name="_AtRisk_SimSetting_RandomNumberGenerator" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_ReportsList" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_SimNameCount" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_StdRecalcBehavior" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStatic" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStaticPercentile" hidden="1">0.5</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="A">[2]不動產!$A$6</definedName>
     <definedName name="aaa">[3]Sheet2!$A$6</definedName>
@@ -37,6 +58,7 @@
     <definedName name="cc">#REF!</definedName>
     <definedName name="CP">#REF!</definedName>
     <definedName name="d">#REF!</definedName>
+    <definedName name="_xlnm.Database" localSheetId="1">#REF!</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
     <definedName name="dfg">'[5]表02(負債業主權益)'!$A$52</definedName>
     <definedName name="DWP">#REF!</definedName>
@@ -86,7 +108,30 @@
     <definedName name="mh">#REF!</definedName>
     <definedName name="netprem_written">[3]Sheet2!#REF!</definedName>
     <definedName name="NWP">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">A142放款餘額彙總表!$B$1:$S$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'表14-2'!$A$1:$K$92</definedName>
+    <definedName name="RiskAfterRecalcMacro" hidden="1">""</definedName>
+    <definedName name="RiskAfterSimMacro" hidden="1">""</definedName>
+    <definedName name="RiskBeforeRecalcMacro" hidden="1">""</definedName>
+    <definedName name="RiskBeforeSimMacro" hidden="1">""</definedName>
+    <definedName name="RiskCollectDistributionSamples" hidden="1">2</definedName>
+    <definedName name="RiskFixedSeed" hidden="1">1</definedName>
+    <definedName name="RiskHasSettings" hidden="1">5</definedName>
+    <definedName name="RiskMinimizeOnStart" hidden="1">FALSE</definedName>
+    <definedName name="RiskMonitorConvergence" hidden="1">FALSE</definedName>
+    <definedName name="RiskNumIterations" hidden="1">10000</definedName>
+    <definedName name="RiskNumSimulations" hidden="1">1</definedName>
+    <definedName name="RiskPauseOnError" hidden="1">FALSE</definedName>
+    <definedName name="RiskRunAfterRecalcMacro" hidden="1">FALSE</definedName>
+    <definedName name="RiskRunAfterSimMacro" hidden="1">FALSE</definedName>
+    <definedName name="RiskRunBeforeRecalcMacro" hidden="1">FALSE</definedName>
+    <definedName name="RiskRunBeforeSimMacro" hidden="1">FALSE</definedName>
+    <definedName name="RiskSamplingType" hidden="1">3</definedName>
+    <definedName name="RiskStandardRecalc" hidden="1">1</definedName>
+    <definedName name="RiskUpdateDisplay" hidden="1">FALSE</definedName>
+    <definedName name="RiskUseDifferentSeedForEachSim" hidden="1">FALSE</definedName>
+    <definedName name="RiskUseFixedSeed" hidden="1">FALSE</definedName>
+    <definedName name="RiskUseMultipleCPUs" hidden="1">FALSE</definedName>
     <definedName name="sencount" hidden="1">3</definedName>
     <definedName name="SHT040BR1">#REF!</definedName>
     <definedName name="SHT040BR2">#REF!</definedName>
@@ -155,12 +200,14 @@
     <definedName name="SHT071TR9">#REF!</definedName>
     <definedName name="SHT080BR1">#REF!</definedName>
     <definedName name="SHT080TR1">#REF!</definedName>
+    <definedName name="SHT100TR8" localSheetId="1">[10]表10!$G$44</definedName>
     <definedName name="SHT100TR8">[5]表10!$G$38</definedName>
     <definedName name="SHT151BR1">#REF!</definedName>
     <definedName name="SHT151TR1">#REF!</definedName>
     <definedName name="sht151tr2">'[5]表15(合併列示及總計)'!$E$7:$E$11</definedName>
     <definedName name="TextRefCopyRangeCount" hidden="1">46</definedName>
     <definedName name="weight_rate">#REF!</definedName>
+    <definedName name="新" localSheetId="1">#REF!</definedName>
     <definedName name="新">#REF!</definedName>
     <definedName name="總體法規稽核結論">#REF!</definedName>
     <definedName name="總體數學勾稽結論">#REF!</definedName>
@@ -170,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="196">
   <si>
     <r>
       <t>新光人壽保險股份有限公司</t>
@@ -1626,12 +1673,407 @@
     </r>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>協理：</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>經理：</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>經辦人：</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Book Antiqua"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">5. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>放款餘額之本金包含折溢價金額。</t>
+    </r>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Book Antiqua"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">4. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>國外：以外幣放款或國際聯貸。</t>
+    </r>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Book Antiqua"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>未列入逾期應予評估放款：包括逾期時間雖尚未達到逾期放款標準，但授信戶已經發生積欠本金或利息的放款；另外，協議分期償還放款雖符合一定條件免予列報逾期放款，仍應列入應予評估放款，不得視為正常之放款。</t>
+    </r>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Book Antiqua"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>逾期：指積欠本金或利息超過清償期三個月，或雖未超過三個月，惟已向主、從債務人訴追或處分擔保品者。協議分期償還放款符合一定條件，並依協議條件履行達六個月以上，且協議利率不低於原承作利率或保險業新承作同類風險放款之利率者，得免予列報逾期放款。
+  但於免列報期間再發生未依約清償超過三個月者，仍應予列報。</t>
+    </r>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>放款種類：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Book Antiqua"/>
+        <family val="1"/>
+      </rPr>
+      <t>A.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>銀行保證放款，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Book Antiqua"/>
+        <family val="1"/>
+      </rPr>
+      <t>B.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>動產擔保放款，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Book Antiqua"/>
+        <family val="1"/>
+      </rPr>
+      <t>C.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>不動產抵押放款，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Book Antiqua"/>
+        <family val="1"/>
+      </rPr>
+      <t>D.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>有價證券質押放款，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Book Antiqua"/>
+        <family val="1"/>
+      </rPr>
+      <t>E.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>壽險貸款，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Book Antiqua"/>
+        <family val="1"/>
+      </rPr>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>墊繳保費，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Book Antiqua"/>
+        <family val="1"/>
+      </rPr>
+      <t>Z.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>其他。</t>
+    </r>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>本表填報定義如下：</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>專案運用</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>TWD</t>
+  </si>
+  <si>
+    <t>TW</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Z</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>備註
+(18)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>IFRS 9預期損失增提金額
+(17)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>備抵損失Ⅴ
+(16)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>備抵損失Ⅳ
+(15)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>備抵損失Ⅲ
+(14)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>備抵損失Ⅱ
+(13)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>備抵損失I
+(12)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>收回無望Ⅴ
+(11)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>收回困難Ⅳ
+(10)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>可望收回Ⅲ
+(9)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>應予注意Ⅱ
+(8)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>正常放款I
+(7)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>未列入逾期應予評估放款
+(6)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>逾期放款
+(5)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否為專案運用公共
+及社會福利事業投資
+(4)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>持有資產幣別
+(3)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>國別
+(2)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>放款種類
+(1)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>單位：新台幣元、%</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>A042放款餘額彙總表</t>
+  </si>
+  <si>
+    <t>報表名稱</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>機密等級：密</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>新光人壽保險股份有限公司</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>公司名稱</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>申報年月</t>
+  </si>
+  <si>
+    <t>報表種類</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>年報</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="20">
+  <numFmts count="22">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -1652,8 +2094,10 @@
     <numFmt numFmtId="190" formatCode="&quot;Yes&quot;;&quot;Yes&quot;;&quot;No&quot;"/>
     <numFmt numFmtId="191" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="192" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="193" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="194" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="71">
+  <fonts count="73">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2136,6 +2580,17 @@
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Book Antiqua"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="38">
@@ -3531,7 +3986,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3821,11 +4276,80 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="4" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="181" fontId="4" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="181" fontId="4" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3865,74 +4389,145 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="71" fillId="0" borderId="0" xfId="165" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="71" fillId="0" borderId="0" xfId="165" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="71" fillId="0" borderId="0" xfId="165" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="193" fontId="71" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="71" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="180" fontId="51" fillId="0" borderId="0" xfId="165" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="22" fillId="0" borderId="0" xfId="89" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="194" fontId="22" fillId="0" borderId="0" xfId="89" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="89" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="194" fontId="8" fillId="0" borderId="20" xfId="165" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="89" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="89" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="51" fillId="0" borderId="10" xfId="165" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="8" fillId="0" borderId="10" xfId="165" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="194" fontId="8" fillId="0" borderId="10" xfId="165" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="194" fontId="8" fillId="0" borderId="20" xfId="165" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="89" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="8" fillId="0" borderId="10" xfId="165" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="8" fillId="0" borderId="10" xfId="165" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="8" fillId="0" borderId="10" xfId="165" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="20" xfId="165" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="20" xfId="165" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="10" xfId="89" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="21" xfId="89" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="288">
@@ -4266,6 +4861,17 @@
       <sheetName val="表30-15"/>
       <sheetName val="表05-1"/>
       <sheetName val="目錄"/>
+      <sheetName val="表03"/>
+      <sheetName val="Q08交易明細"/>
+      <sheetName val="表30-13-1"/>
+      <sheetName val="表07(總計)"/>
+      <sheetName val="表06"/>
+      <sheetName val="封面"/>
+      <sheetName val="03ws"/>
+      <sheetName val="非認許A"/>
+      <sheetName val="備供累計"/>
+      <sheetName val="Reserve"/>
+      <sheetName val="工作表2"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -4292,6 +4898,124 @@
       <sheetData sheetId="21" refreshError="1"/>
       <sheetData sheetId="22" refreshError="1"/>
       <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="封面"/>
+      <sheetName val="公司基本資料"/>
+      <sheetName val="公司動態基本資料"/>
+      <sheetName val="表01"/>
+      <sheetName val="表02(資產)"/>
+      <sheetName val="表02(資產附表)"/>
+      <sheetName val="表02(負債業主權益)"/>
+      <sheetName val="表03"/>
+      <sheetName val="表04"/>
+      <sheetName val="表05(個人契約)"/>
+      <sheetName val="表05(團體契約)"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="表06"/>
+      <sheetName val="表07(個人契約)"/>
+      <sheetName val="表07(團體契約)"/>
+      <sheetName val="表08"/>
+      <sheetName val="表09"/>
+      <sheetName val="表10"/>
+      <sheetName val="表11"/>
+      <sheetName val="表11(總計)"/>
+      <sheetName val="表12"/>
+      <sheetName val="表13"/>
+      <sheetName val="表13(總計)"/>
+      <sheetName val="表14"/>
+      <sheetName val="表14(總計)"/>
+      <sheetName val="表15"/>
+      <sheetName val="表15(合併列示及總計)"/>
+      <sheetName val="表16"/>
+      <sheetName val="表16(總計)"/>
+      <sheetName val="表17"/>
+      <sheetName val="表17(總計)"/>
+      <sheetName val="表18"/>
+      <sheetName val="表18(總計)"/>
+      <sheetName val="表19"/>
+      <sheetName val="表19-1"/>
+      <sheetName val="表20"/>
+      <sheetName val="表20(總計)"/>
+      <sheetName val="表21"/>
+      <sheetName val="格式檢查"/>
+      <sheetName val="數學勾稽"/>
+      <sheetName val="轉檔資訊"/>
+      <sheetName val="適法性稽核"/>
+      <sheetName val="合理性稽核"/>
+      <sheetName val="引申變數"/>
+      <sheetName val="代碼資料"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17">
+        <row r="44">
+          <cell r="G44">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6689,6 +7413,21 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="A042填報說明"/>
+      <sheetName val="A042放款餘額彙總表"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
@@ -6982,7 +7721,7 @@
   <dimension ref="A1:Y116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
@@ -7022,11 +7761,11 @@
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -7040,39 +7779,39 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:13" s="7" customFormat="1">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="116" t="s">
+      <c r="C3" s="133"/>
+      <c r="D3" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="127" t="s">
+      <c r="E3" s="139"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="118" t="s">
+      <c r="H3" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="118" t="s">
+      <c r="I3" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="120" t="s">
+      <c r="J3" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="122" t="s">
+      <c r="K3" s="119" t="s">
         <v>10</v>
       </c>
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:13" s="7" customFormat="1">
-      <c r="A4" s="109"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="113"/>
+      <c r="A4" s="131"/>
+      <c r="B4" s="134"/>
+      <c r="C4" s="135"/>
       <c r="D4" s="10" t="s">
         <v>11</v>
       </c>
@@ -7082,17 +7821,17 @@
       <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="128"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="121"/>
-      <c r="K4" s="123"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="120"/>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:13" s="7" customFormat="1">
-      <c r="A5" s="109"/>
-      <c r="B5" s="114"/>
-      <c r="C5" s="115"/>
+      <c r="A5" s="131"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="137"/>
       <c r="D5" s="12" t="s">
         <v>14</v>
       </c>
@@ -7124,7 +7863,7 @@
       <c r="A6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="121" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -7158,7 +7897,7 @@
       <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="125"/>
+      <c r="B7" s="122"/>
       <c r="C7" s="17" t="s">
         <v>27</v>
       </c>
@@ -7196,7 +7935,7 @@
       <c r="A8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="105"/>
+      <c r="B8" s="123"/>
       <c r="C8" s="26" t="s">
         <v>30</v>
       </c>
@@ -7226,7 +7965,7 @@
       <c r="A9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="105"/>
+      <c r="B9" s="123"/>
       <c r="C9" s="26" t="s">
         <v>32</v>
       </c>
@@ -7253,7 +7992,7 @@
       <c r="A10" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="105"/>
+      <c r="B10" s="123"/>
       <c r="C10" s="26" t="s">
         <v>34</v>
       </c>
@@ -7280,7 +8019,7 @@
       <c r="A11" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="105"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="26" t="s">
         <v>36</v>
       </c>
@@ -7307,7 +8046,7 @@
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="105"/>
+      <c r="B12" s="123"/>
       <c r="C12" s="32" t="s">
         <v>38</v>
       </c>
@@ -7334,7 +8073,7 @@
       <c r="A13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="105"/>
+      <c r="B13" s="123"/>
       <c r="C13" s="32" t="s">
         <v>40</v>
       </c>
@@ -7370,7 +8109,7 @@
       <c r="A14" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="124" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="26" t="s">
@@ -7399,7 +8138,7 @@
       <c r="A15" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="105"/>
+      <c r="B15" s="123"/>
       <c r="C15" s="26" t="s">
         <v>45</v>
       </c>
@@ -7426,7 +8165,7 @@
       <c r="A16" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="105"/>
+      <c r="B16" s="123"/>
       <c r="C16" s="26" t="s">
         <v>47</v>
       </c>
@@ -7453,7 +8192,7 @@
       <c r="A17" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="126"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="37" t="s">
         <v>49</v>
       </c>
@@ -7479,7 +8218,7 @@
       <c r="A18" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="126"/>
+      <c r="B18" s="125"/>
       <c r="C18" s="37" t="s">
         <v>40</v>
       </c>
@@ -7514,7 +8253,7 @@
       <c r="A19" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="104" t="s">
+      <c r="B19" s="124" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="26" t="s">
@@ -7542,7 +8281,7 @@
       <c r="A20" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="105"/>
+      <c r="B20" s="123"/>
       <c r="C20" s="26" t="s">
         <v>45</v>
       </c>
@@ -7568,7 +8307,7 @@
       <c r="A21" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="105"/>
+      <c r="B21" s="123"/>
       <c r="C21" s="26" t="s">
         <v>47</v>
       </c>
@@ -7594,7 +8333,7 @@
       <c r="A22" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="105"/>
+      <c r="B22" s="123"/>
       <c r="C22" s="37" t="s">
         <v>49</v>
       </c>
@@ -7620,7 +8359,7 @@
       <c r="A23" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="134" t="s">
+      <c r="B23" s="109" t="s">
         <v>57</v>
       </c>
       <c r="C23" s="37" t="s">
@@ -7657,7 +8396,7 @@
       <c r="A24" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="135"/>
+      <c r="B24" s="110"/>
       <c r="C24" s="37" t="s">
         <v>60</v>
       </c>
@@ -7683,7 +8422,7 @@
       <c r="A25" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="134" t="s">
+      <c r="B25" s="109" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="26" t="s">
@@ -7720,7 +8459,7 @@
       <c r="A26" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="136"/>
+      <c r="B26" s="111"/>
       <c r="C26" s="38" t="s">
         <v>64</v>
       </c>
@@ -7746,7 +8485,7 @@
       <c r="A27" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="136"/>
+      <c r="B27" s="111"/>
       <c r="C27" s="38" t="s">
         <v>66</v>
       </c>
@@ -7772,7 +8511,7 @@
       <c r="A28" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="136"/>
+      <c r="B28" s="111"/>
       <c r="C28" s="38" t="s">
         <v>68</v>
       </c>
@@ -7798,7 +8537,7 @@
       <c r="A29" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="136"/>
+      <c r="B29" s="111"/>
       <c r="C29" s="38" t="s">
         <v>70</v>
       </c>
@@ -7824,7 +8563,7 @@
       <c r="A30" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="136"/>
+      <c r="B30" s="111"/>
       <c r="C30" s="38" t="s">
         <v>72</v>
       </c>
@@ -7850,7 +8589,7 @@
       <c r="A31" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="136"/>
+      <c r="B31" s="111"/>
       <c r="C31" s="26" t="s">
         <v>27</v>
       </c>
@@ -7885,7 +8624,7 @@
       <c r="A32" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="136"/>
+      <c r="B32" s="111"/>
       <c r="C32" s="38" t="s">
         <v>64</v>
       </c>
@@ -7911,7 +8650,7 @@
       <c r="A33" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="136"/>
+      <c r="B33" s="111"/>
       <c r="C33" s="38" t="s">
         <v>66</v>
       </c>
@@ -7938,7 +8677,7 @@
       <c r="A34" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="136"/>
+      <c r="B34" s="111"/>
       <c r="C34" s="38" t="s">
         <v>68</v>
       </c>
@@ -7965,7 +8704,7 @@
       <c r="A35" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="136"/>
+      <c r="B35" s="111"/>
       <c r="C35" s="38" t="s">
         <v>70</v>
       </c>
@@ -7992,7 +8731,7 @@
       <c r="A36" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="136"/>
+      <c r="B36" s="111"/>
       <c r="C36" s="38" t="s">
         <v>72</v>
       </c>
@@ -8019,7 +8758,7 @@
       <c r="A37" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="136"/>
+      <c r="B37" s="111"/>
       <c r="C37" s="26" t="s">
         <v>30</v>
       </c>
@@ -8055,7 +8794,7 @@
       <c r="A38" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="136"/>
+      <c r="B38" s="111"/>
       <c r="C38" s="38" t="s">
         <v>64</v>
       </c>
@@ -8082,7 +8821,7 @@
       <c r="A39" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="136"/>
+      <c r="B39" s="111"/>
       <c r="C39" s="38" t="s">
         <v>66</v>
       </c>
@@ -8109,7 +8848,7 @@
       <c r="A40" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="136"/>
+      <c r="B40" s="111"/>
       <c r="C40" s="38" t="s">
         <v>68</v>
       </c>
@@ -8136,7 +8875,7 @@
       <c r="A41" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="136"/>
+      <c r="B41" s="111"/>
       <c r="C41" s="38" t="s">
         <v>70</v>
       </c>
@@ -8163,7 +8902,7 @@
       <c r="A42" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="136"/>
+      <c r="B42" s="111"/>
       <c r="C42" s="38" t="s">
         <v>72</v>
       </c>
@@ -8190,7 +8929,7 @@
       <c r="A43" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="136"/>
+      <c r="B43" s="111"/>
       <c r="C43" s="26" t="s">
         <v>86</v>
       </c>
@@ -8226,7 +8965,7 @@
       <c r="A44" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="136"/>
+      <c r="B44" s="111"/>
       <c r="C44" s="38" t="s">
         <v>64</v>
       </c>
@@ -8253,7 +8992,7 @@
       <c r="A45" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="136"/>
+      <c r="B45" s="111"/>
       <c r="C45" s="38" t="s">
         <v>66</v>
       </c>
@@ -8280,7 +9019,7 @@
       <c r="A46" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="136"/>
+      <c r="B46" s="111"/>
       <c r="C46" s="38" t="s">
         <v>68</v>
       </c>
@@ -8307,7 +9046,7 @@
       <c r="A47" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="136"/>
+      <c r="B47" s="111"/>
       <c r="C47" s="38" t="s">
         <v>70</v>
       </c>
@@ -8334,7 +9073,7 @@
       <c r="A48" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="136"/>
+      <c r="B48" s="111"/>
       <c r="C48" s="38" t="s">
         <v>72</v>
       </c>
@@ -8361,7 +9100,7 @@
       <c r="A49" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="136"/>
+      <c r="B49" s="111"/>
       <c r="C49" s="26" t="s">
         <v>34</v>
       </c>
@@ -8396,7 +9135,7 @@
       <c r="A50" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="136"/>
+      <c r="B50" s="111"/>
       <c r="C50" s="38" t="s">
         <v>64</v>
       </c>
@@ -8422,7 +9161,7 @@
       <c r="A51" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="136"/>
+      <c r="B51" s="111"/>
       <c r="C51" s="38" t="s">
         <v>66</v>
       </c>
@@ -8448,7 +9187,7 @@
       <c r="A52" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="136"/>
+      <c r="B52" s="111"/>
       <c r="C52" s="38" t="s">
         <v>96</v>
       </c>
@@ -8474,7 +9213,7 @@
       <c r="A53" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B53" s="136"/>
+      <c r="B53" s="111"/>
       <c r="C53" s="38" t="s">
         <v>70</v>
       </c>
@@ -8500,7 +9239,7 @@
       <c r="A54" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="136"/>
+      <c r="B54" s="111"/>
       <c r="C54" s="38" t="s">
         <v>72</v>
       </c>
@@ -8526,7 +9265,7 @@
       <c r="A55" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B55" s="136"/>
+      <c r="B55" s="111"/>
       <c r="C55" s="26" t="s">
         <v>36</v>
       </c>
@@ -8561,7 +9300,7 @@
       <c r="A56" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B56" s="136"/>
+      <c r="B56" s="111"/>
       <c r="C56" s="38" t="s">
         <v>64</v>
       </c>
@@ -8587,7 +9326,7 @@
       <c r="A57" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="136"/>
+      <c r="B57" s="111"/>
       <c r="C57" s="38" t="s">
         <v>66</v>
       </c>
@@ -8613,7 +9352,7 @@
       <c r="A58" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B58" s="136"/>
+      <c r="B58" s="111"/>
       <c r="C58" s="38" t="s">
         <v>68</v>
       </c>
@@ -8639,7 +9378,7 @@
       <c r="A59" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B59" s="136"/>
+      <c r="B59" s="111"/>
       <c r="C59" s="38" t="s">
         <v>70</v>
       </c>
@@ -8665,7 +9404,7 @@
       <c r="A60" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B60" s="136"/>
+      <c r="B60" s="111"/>
       <c r="C60" s="38" t="s">
         <v>72</v>
       </c>
@@ -8691,7 +9430,7 @@
       <c r="A61" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="136"/>
+      <c r="B61" s="111"/>
       <c r="C61" s="32" t="s">
         <v>38</v>
       </c>
@@ -8726,7 +9465,7 @@
       <c r="A62" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B62" s="136"/>
+      <c r="B62" s="111"/>
       <c r="C62" s="38" t="s">
         <v>64</v>
       </c>
@@ -8752,7 +9491,7 @@
       <c r="A63" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B63" s="136"/>
+      <c r="B63" s="111"/>
       <c r="C63" s="38" t="s">
         <v>66</v>
       </c>
@@ -8778,7 +9517,7 @@
       <c r="A64" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B64" s="136"/>
+      <c r="B64" s="111"/>
       <c r="C64" s="38" t="s">
         <v>68</v>
       </c>
@@ -8804,7 +9543,7 @@
       <c r="A65" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B65" s="136"/>
+      <c r="B65" s="111"/>
       <c r="C65" s="38" t="s">
         <v>70</v>
       </c>
@@ -8836,7 +9575,7 @@
       <c r="A66" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="136"/>
+      <c r="B66" s="111"/>
       <c r="C66" s="38" t="s">
         <v>72</v>
       </c>
@@ -8868,10 +9607,10 @@
       <c r="A67" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="B67" s="129" t="s">
+      <c r="B67" s="104" t="s">
         <v>112</v>
       </c>
-      <c r="C67" s="130"/>
+      <c r="C67" s="105"/>
       <c r="D67" s="30">
         <f>D61+D55+D23</f>
         <v>0</v>
@@ -8909,10 +9648,10 @@
       <c r="A68" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B68" s="129" t="s">
+      <c r="B68" s="104" t="s">
         <v>114</v>
       </c>
-      <c r="C68" s="130"/>
+      <c r="C68" s="105"/>
       <c r="D68" s="30"/>
       <c r="E68" s="30"/>
       <c r="F68" s="93" t="e">
@@ -8941,10 +9680,10 @@
       <c r="A69" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B69" s="129" t="s">
+      <c r="B69" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="C69" s="130"/>
+      <c r="C69" s="105"/>
       <c r="D69" s="30">
         <f>$D$25+$D$31+$D$37+$D$43+$D$49</f>
         <v>0</v>
@@ -8982,17 +9721,17 @@
       <c r="A70" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B70" s="129" t="s">
+      <c r="B70" s="104" t="s">
         <v>118</v>
       </c>
-      <c r="C70" s="130"/>
-      <c r="D70" s="137"/>
-      <c r="E70" s="138"/>
-      <c r="F70" s="138"/>
-      <c r="G70" s="138"/>
-      <c r="H70" s="138"/>
-      <c r="I70" s="138"/>
-      <c r="J70" s="139"/>
+      <c r="C70" s="105"/>
+      <c r="D70" s="112"/>
+      <c r="E70" s="113"/>
+      <c r="F70" s="113"/>
+      <c r="G70" s="113"/>
+      <c r="H70" s="113"/>
+      <c r="I70" s="113"/>
+      <c r="J70" s="114"/>
       <c r="K70" s="18"/>
       <c r="L70" s="45"/>
       <c r="M70" s="42"/>
@@ -9005,17 +9744,17 @@
       <c r="A71" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B71" s="129" t="s">
+      <c r="B71" s="104" t="s">
         <v>120</v>
       </c>
-      <c r="C71" s="130"/>
-      <c r="D71" s="137"/>
-      <c r="E71" s="138"/>
-      <c r="F71" s="138"/>
-      <c r="G71" s="138"/>
-      <c r="H71" s="138"/>
-      <c r="I71" s="138"/>
-      <c r="J71" s="139"/>
+      <c r="C71" s="105"/>
+      <c r="D71" s="112"/>
+      <c r="E71" s="113"/>
+      <c r="F71" s="113"/>
+      <c r="G71" s="113"/>
+      <c r="H71" s="113"/>
+      <c r="I71" s="113"/>
+      <c r="J71" s="114"/>
       <c r="K71" s="18"/>
       <c r="L71" s="46"/>
       <c r="M71" s="44"/>
@@ -9028,20 +9767,20 @@
       <c r="A72" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="B72" s="129" t="s">
+      <c r="B72" s="104" t="s">
         <v>122</v>
       </c>
-      <c r="C72" s="130"/>
-      <c r="D72" s="131" t="e">
+      <c r="C72" s="105"/>
+      <c r="D72" s="106" t="e">
         <f>D70/H67</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E72" s="132"/>
-      <c r="F72" s="132"/>
-      <c r="G72" s="132"/>
-      <c r="H72" s="132"/>
-      <c r="I72" s="132"/>
-      <c r="J72" s="133"/>
+      <c r="E72" s="107"/>
+      <c r="F72" s="107"/>
+      <c r="G72" s="107"/>
+      <c r="H72" s="107"/>
+      <c r="I72" s="107"/>
+      <c r="J72" s="108"/>
       <c r="K72" s="18"/>
       <c r="L72" s="44"/>
       <c r="M72" s="42"/>
@@ -9054,20 +9793,20 @@
       <c r="A73" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B73" s="129" t="s">
+      <c r="B73" s="104" t="s">
         <v>124</v>
       </c>
-      <c r="C73" s="130"/>
-      <c r="D73" s="131" t="e">
+      <c r="C73" s="105"/>
+      <c r="D73" s="106" t="e">
         <f>D71/H67</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E73" s="132"/>
-      <c r="F73" s="132"/>
-      <c r="G73" s="132"/>
-      <c r="H73" s="132"/>
-      <c r="I73" s="132"/>
-      <c r="J73" s="133"/>
+      <c r="E73" s="107"/>
+      <c r="F73" s="107"/>
+      <c r="G73" s="107"/>
+      <c r="H73" s="107"/>
+      <c r="I73" s="107"/>
+      <c r="J73" s="108"/>
       <c r="K73" s="18"/>
       <c r="L73" s="42"/>
       <c r="M73" s="42"/>
@@ -9080,20 +9819,20 @@
       <c r="A74" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B74" s="129" t="s">
+      <c r="B74" s="104" t="s">
         <v>126</v>
       </c>
-      <c r="C74" s="130"/>
-      <c r="D74" s="131" t="e">
+      <c r="C74" s="105"/>
+      <c r="D74" s="106" t="e">
         <f>(D70+D71)/H67</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E74" s="132"/>
-      <c r="F74" s="132"/>
-      <c r="G74" s="132"/>
-      <c r="H74" s="132"/>
-      <c r="I74" s="132"/>
-      <c r="J74" s="133"/>
+      <c r="E74" s="107"/>
+      <c r="F74" s="107"/>
+      <c r="G74" s="107"/>
+      <c r="H74" s="107"/>
+      <c r="I74" s="107"/>
+      <c r="J74" s="108"/>
       <c r="K74" s="18"/>
       <c r="L74" s="42"/>
       <c r="M74" s="7"/>
@@ -9106,20 +9845,20 @@
       <c r="A75" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B75" s="129" t="s">
+      <c r="B75" s="104" t="s">
         <v>128</v>
       </c>
-      <c r="C75" s="130"/>
-      <c r="D75" s="131" t="e">
+      <c r="C75" s="105"/>
+      <c r="D75" s="106" t="e">
         <f>D70/H69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E75" s="132"/>
-      <c r="F75" s="132"/>
-      <c r="G75" s="132"/>
-      <c r="H75" s="132"/>
-      <c r="I75" s="132"/>
-      <c r="J75" s="133"/>
+      <c r="E75" s="107"/>
+      <c r="F75" s="107"/>
+      <c r="G75" s="107"/>
+      <c r="H75" s="107"/>
+      <c r="I75" s="107"/>
+      <c r="J75" s="108"/>
       <c r="K75" s="18"/>
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
@@ -9132,20 +9871,20 @@
       <c r="A76" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B76" s="129" t="s">
+      <c r="B76" s="104" t="s">
         <v>130</v>
       </c>
-      <c r="C76" s="130"/>
-      <c r="D76" s="131" t="e">
+      <c r="C76" s="105"/>
+      <c r="D76" s="106" t="e">
         <f>D71/H69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E76" s="132"/>
-      <c r="F76" s="132"/>
-      <c r="G76" s="132"/>
-      <c r="H76" s="132"/>
-      <c r="I76" s="132"/>
-      <c r="J76" s="133"/>
+      <c r="E76" s="107"/>
+      <c r="F76" s="107"/>
+      <c r="G76" s="107"/>
+      <c r="H76" s="107"/>
+      <c r="I76" s="107"/>
+      <c r="J76" s="108"/>
       <c r="K76" s="18"/>
       <c r="L76" s="7"/>
       <c r="M76" s="7"/>
@@ -9158,20 +9897,20 @@
       <c r="A77" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B77" s="129" t="s">
+      <c r="B77" s="104" t="s">
         <v>132</v>
       </c>
-      <c r="C77" s="130"/>
-      <c r="D77" s="131" t="e">
+      <c r="C77" s="105"/>
+      <c r="D77" s="106" t="e">
         <f>(F70+F71)/H69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E77" s="132"/>
-      <c r="F77" s="132"/>
-      <c r="G77" s="132"/>
-      <c r="H77" s="132"/>
-      <c r="I77" s="132"/>
-      <c r="J77" s="133"/>
+      <c r="E77" s="107"/>
+      <c r="F77" s="107"/>
+      <c r="G77" s="107"/>
+      <c r="H77" s="107"/>
+      <c r="I77" s="107"/>
+      <c r="J77" s="108"/>
       <c r="K77" s="18"/>
       <c r="L77" s="7"/>
       <c r="M77" s="7"/>
@@ -9371,7 +10110,7 @@
         <v>0</v>
       </c>
       <c r="E85" s="61">
-        <f t="shared" ref="E84:F87" si="5">H40*10%</f>
+        <f t="shared" ref="E85" si="5">H40*10%</f>
         <v>0</v>
       </c>
       <c r="F85" s="61">
@@ -9514,7 +10253,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="73">
-        <f t="shared" ref="D88:I88" si="6">SUM(F83:F87)</f>
+        <f t="shared" ref="F88:I88" si="6">SUM(F83:F87)</f>
         <v>0</v>
       </c>
       <c r="G88" s="73">
@@ -9633,14 +10372,18 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="D77:J77"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:J74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:J75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:J76"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="D73:J73"/>
     <mergeCell ref="B23:B24"/>
@@ -9654,22 +10397,555 @@
     <mergeCell ref="D71:J71"/>
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="D72:J72"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:C5"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="D77:J77"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:J74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:J75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:J76"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="0.35433070866141736" bottom="0.35433070866141736" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="56" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Y22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="7" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="2.90625" style="140" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" style="140" customWidth="1"/>
+    <col min="3" max="3" width="9" style="140" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" style="140" customWidth="1"/>
+    <col min="5" max="5" width="21.36328125" style="140" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" style="140" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" style="140" customWidth="1"/>
+    <col min="8" max="8" width="24.90625" style="140" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" style="140" customWidth="1"/>
+    <col min="10" max="10" width="21.453125" style="140" customWidth="1"/>
+    <col min="11" max="12" width="12.6328125" style="140" customWidth="1"/>
+    <col min="13" max="13" width="17.90625" style="140" customWidth="1"/>
+    <col min="14" max="15" width="17.36328125" style="140" customWidth="1"/>
+    <col min="16" max="17" width="15.6328125" style="140" customWidth="1"/>
+    <col min="18" max="18" width="24.1796875" style="140" customWidth="1"/>
+    <col min="19" max="19" width="12.90625" style="140" customWidth="1"/>
+    <col min="20" max="16384" width="9" style="140"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:24">
+      <c r="B1" s="140" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="140" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="2:24">
+      <c r="B2" s="140" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="186">
+        <v>201909</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24">
+      <c r="B3" s="140" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="182" t="s">
+        <v>191</v>
+      </c>
+      <c r="R3" s="185"/>
+      <c r="S3" s="185" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24">
+      <c r="B4" s="140" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="182" t="s">
+        <v>188</v>
+      </c>
+      <c r="R4" s="184"/>
+      <c r="S4" s="183" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24">
+      <c r="C5" s="182"/>
+      <c r="R5" s="184"/>
+      <c r="S5" s="183"/>
+    </row>
+    <row r="6" spans="2:24">
+      <c r="C6" s="182"/>
+      <c r="R6" s="181"/>
+      <c r="S6" s="181"/>
+    </row>
+    <row r="7" spans="2:24" s="179" customFormat="1" ht="51">
+      <c r="B7" s="180" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="180" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="180" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" s="180" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="180" t="s">
+        <v>182</v>
+      </c>
+      <c r="G7" s="180" t="s">
+        <v>181</v>
+      </c>
+      <c r="H7" s="180" t="s">
+        <v>180</v>
+      </c>
+      <c r="I7" s="180" t="s">
+        <v>179</v>
+      </c>
+      <c r="J7" s="180" t="s">
+        <v>178</v>
+      </c>
+      <c r="K7" s="180" t="s">
+        <v>177</v>
+      </c>
+      <c r="L7" s="180" t="s">
+        <v>176</v>
+      </c>
+      <c r="M7" s="180" t="s">
+        <v>175</v>
+      </c>
+      <c r="N7" s="180" t="s">
+        <v>174</v>
+      </c>
+      <c r="O7" s="180" t="s">
+        <v>173</v>
+      </c>
+      <c r="P7" s="180" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q7" s="180" t="s">
+        <v>171</v>
+      </c>
+      <c r="R7" s="180" t="s">
+        <v>170</v>
+      </c>
+      <c r="S7" s="180" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" s="176" customFormat="1" ht="15.5">
+      <c r="B8" s="167" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="167" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="167" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" s="166" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" s="171"/>
+      <c r="G8" s="171"/>
+      <c r="H8" s="171"/>
+      <c r="I8" s="171"/>
+      <c r="J8" s="171"/>
+      <c r="K8" s="171"/>
+      <c r="L8" s="171"/>
+      <c r="M8" s="171"/>
+      <c r="N8" s="171"/>
+      <c r="O8" s="171"/>
+      <c r="P8" s="171"/>
+      <c r="Q8" s="171"/>
+      <c r="R8" s="178"/>
+      <c r="S8" s="177"/>
+    </row>
+    <row r="9" spans="2:24" s="176" customFormat="1" ht="15.5">
+      <c r="B9" s="167" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="167" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="167" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" s="166" t="s">
+        <v>164</v>
+      </c>
+      <c r="F9" s="171"/>
+      <c r="G9" s="171"/>
+      <c r="H9" s="171"/>
+      <c r="I9" s="171"/>
+      <c r="J9" s="171"/>
+      <c r="K9" s="171"/>
+      <c r="L9" s="171"/>
+      <c r="M9" s="171"/>
+      <c r="N9" s="171"/>
+      <c r="O9" s="171"/>
+      <c r="P9" s="171"/>
+      <c r="Q9" s="171"/>
+      <c r="R9" s="178"/>
+      <c r="S9" s="177"/>
+    </row>
+    <row r="10" spans="2:24" s="163" customFormat="1" ht="15.5">
+      <c r="B10" s="167" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="167" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="167" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" s="166" t="s">
+        <v>164</v>
+      </c>
+      <c r="F10" s="165"/>
+      <c r="G10" s="165"/>
+      <c r="H10" s="165"/>
+      <c r="I10" s="165"/>
+      <c r="J10" s="165"/>
+      <c r="K10" s="171"/>
+      <c r="L10" s="165"/>
+      <c r="M10" s="165"/>
+      <c r="N10" s="165"/>
+      <c r="O10" s="165"/>
+      <c r="P10" s="165"/>
+      <c r="Q10" s="170"/>
+      <c r="R10" s="175"/>
+      <c r="S10" s="174"/>
+    </row>
+    <row r="11" spans="2:24" s="163" customFormat="1" ht="15.5">
+      <c r="B11" s="167" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="167" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="167" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" s="166" t="s">
+        <v>164</v>
+      </c>
+      <c r="F11" s="165"/>
+      <c r="G11" s="165"/>
+      <c r="H11" s="165"/>
+      <c r="I11" s="165"/>
+      <c r="J11" s="165"/>
+      <c r="K11" s="171"/>
+      <c r="L11" s="165"/>
+      <c r="M11" s="165"/>
+      <c r="N11" s="165"/>
+      <c r="O11" s="165"/>
+      <c r="P11" s="165"/>
+      <c r="Q11" s="170"/>
+      <c r="R11" s="169"/>
+      <c r="S11" s="173"/>
+    </row>
+    <row r="12" spans="2:24" s="163" customFormat="1">
+      <c r="B12" s="167" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="167" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="167" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" s="172" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" s="165"/>
+      <c r="G12" s="165"/>
+      <c r="H12" s="165"/>
+      <c r="I12" s="165"/>
+      <c r="J12" s="165"/>
+      <c r="K12" s="171"/>
+      <c r="L12" s="165"/>
+      <c r="M12" s="165"/>
+      <c r="N12" s="165"/>
+      <c r="O12" s="165"/>
+      <c r="P12" s="165"/>
+      <c r="Q12" s="170"/>
+      <c r="R12" s="169"/>
+      <c r="S12" s="168" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" s="163" customFormat="1" ht="15.5">
+      <c r="B13" s="167"/>
+      <c r="C13" s="167"/>
+      <c r="D13" s="167"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="164"/>
+      <c r="G13" s="164"/>
+      <c r="H13" s="165"/>
+      <c r="I13" s="164"/>
+      <c r="J13" s="164"/>
+      <c r="K13" s="164"/>
+      <c r="L13" s="164"/>
+      <c r="M13" s="164"/>
+      <c r="N13" s="164"/>
+      <c r="O13" s="164"/>
+      <c r="P13" s="164"/>
+      <c r="Q13" s="164"/>
+      <c r="R13" s="164"/>
+      <c r="S13" s="164"/>
+    </row>
+    <row r="14" spans="2:24" s="160" customFormat="1">
+      <c r="F14" s="162">
+        <f>SUM(F8:F13)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="162">
+        <f>SUM(G8:G13)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="162">
+        <f>SUM(H8:H13)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="162">
+        <f>SUM(I8:I13)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="162">
+        <f>SUM(J8:J13)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="162">
+        <f>SUM(K8:K13)</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="162">
+        <f>SUM(L8:L13)</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="162">
+        <f>SUM(M8:M13)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="162">
+        <f>SUM(N8:N13)</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="162">
+        <f>SUM(O8:O13)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="162">
+        <f>SUM(P8:P13)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="162">
+        <f>SUM(Q8:Q13)</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="161"/>
+    </row>
+    <row r="15" spans="2:24">
+      <c r="B15" s="152" t="s">
+        <v>158</v>
+      </c>
+      <c r="C15" s="158"/>
+      <c r="D15" s="158"/>
+      <c r="E15" s="159"/>
+      <c r="F15" s="158"/>
+      <c r="G15" s="152"/>
+      <c r="H15" s="152"/>
+      <c r="I15" s="152"/>
+      <c r="J15" s="152"/>
+      <c r="K15" s="152"/>
+      <c r="L15" s="152"/>
+      <c r="M15" s="157"/>
+      <c r="N15" s="157"/>
+      <c r="O15" s="157"/>
+      <c r="P15" s="157"/>
+      <c r="Q15" s="157"/>
+      <c r="R15" s="152"/>
+      <c r="S15" s="152"/>
+      <c r="T15" s="152"/>
+      <c r="U15" s="152"/>
+      <c r="V15" s="152"/>
+      <c r="W15" s="152"/>
+      <c r="X15" s="152"/>
+    </row>
+    <row r="16" spans="2:24">
+      <c r="B16" s="156" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="153"/>
+      <c r="I16" s="152"/>
+      <c r="J16" s="152"/>
+      <c r="K16" s="152"/>
+      <c r="L16" s="152"/>
+      <c r="M16" s="152"/>
+      <c r="N16" s="152"/>
+      <c r="O16" s="152"/>
+      <c r="P16" s="152"/>
+      <c r="Q16" s="152"/>
+      <c r="R16" s="152"/>
+      <c r="S16" s="152"/>
+      <c r="T16" s="152"/>
+      <c r="U16" s="152"/>
+      <c r="V16" s="152"/>
+      <c r="W16" s="152"/>
+      <c r="X16" s="152"/>
+    </row>
+    <row r="17" spans="1:25" ht="35.25" customHeight="1">
+      <c r="B17" s="154" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" s="154"/>
+      <c r="D17" s="154"/>
+      <c r="E17" s="154"/>
+      <c r="F17" s="154"/>
+      <c r="G17" s="154"/>
+      <c r="H17" s="154"/>
+      <c r="I17" s="154"/>
+      <c r="J17" s="154"/>
+      <c r="K17" s="154"/>
+      <c r="L17" s="154"/>
+      <c r="M17" s="154"/>
+      <c r="N17" s="154"/>
+      <c r="O17" s="154"/>
+      <c r="P17" s="154"/>
+      <c r="Q17" s="154"/>
+      <c r="R17" s="154"/>
+      <c r="S17" s="154"/>
+      <c r="T17" s="153"/>
+      <c r="U17" s="153"/>
+      <c r="V17" s="153"/>
+      <c r="W17" s="153"/>
+      <c r="X17" s="153"/>
+    </row>
+    <row r="18" spans="1:25" ht="16.5" customHeight="1">
+      <c r="B18" s="154" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="154"/>
+      <c r="D18" s="154"/>
+      <c r="E18" s="154"/>
+      <c r="F18" s="154"/>
+      <c r="G18" s="154"/>
+      <c r="H18" s="154"/>
+      <c r="I18" s="154"/>
+      <c r="J18" s="154"/>
+      <c r="K18" s="154"/>
+      <c r="L18" s="154"/>
+      <c r="M18" s="154"/>
+      <c r="N18" s="154"/>
+      <c r="O18" s="154"/>
+      <c r="P18" s="154"/>
+      <c r="Q18" s="154"/>
+      <c r="R18" s="154"/>
+      <c r="S18" s="153"/>
+      <c r="T18" s="153"/>
+      <c r="U18" s="153"/>
+      <c r="V18" s="153"/>
+      <c r="W18" s="153"/>
+      <c r="X18" s="153"/>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="B19" s="152" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19" s="152"/>
+      <c r="D19" s="152"/>
+      <c r="E19" s="152"/>
+      <c r="F19" s="152"/>
+      <c r="G19" s="152"/>
+      <c r="H19" s="152"/>
+      <c r="I19" s="152"/>
+      <c r="J19" s="152"/>
+      <c r="K19" s="152"/>
+      <c r="L19" s="152"/>
+      <c r="M19" s="152"/>
+      <c r="N19" s="152"/>
+      <c r="O19" s="152"/>
+      <c r="P19" s="152"/>
+      <c r="Q19" s="152"/>
+      <c r="R19" s="152"/>
+      <c r="S19" s="152"/>
+      <c r="T19" s="152"/>
+      <c r="U19" s="152"/>
+      <c r="V19" s="152"/>
+      <c r="W19" s="152"/>
+      <c r="X19" s="152"/>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="B20" s="140" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" s="141" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A22" s="151"/>
+      <c r="B22" s="141" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="150"/>
+      <c r="D22" s="147"/>
+      <c r="G22" s="146"/>
+      <c r="I22" s="146" t="s">
+        <v>151</v>
+      </c>
+      <c r="J22" s="148"/>
+      <c r="K22" s="149"/>
+      <c r="M22" s="148"/>
+      <c r="N22" s="147"/>
+      <c r="O22" s="146"/>
+      <c r="P22" s="141" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q22" s="145"/>
+      <c r="R22" s="144"/>
+      <c r="T22" s="143"/>
+      <c r="W22" s="142"/>
+      <c r="Y22" s="141" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B17:S17"/>
+    <mergeCell ref="B18:R18"/>
+    <mergeCell ref="R6:S6"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="47" orientation="landscape" horizontalDpi="4294967294" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"標楷體,標準"&amp;14製表單位：放款管理課&amp;C第 &amp;P 頁，共 &amp;N 頁</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>